<commit_message>
Update vaccination for april 14 calender
</commit_message>
<xml_diff>
--- a/data/Vaccine prognoser (jan-juli).xlsx
+++ b/data/Vaccine prognoser (jan-juli).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alboa\Documents\GitHub\covid-19-modelling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C10407F-748D-454E-B4EC-CF6700A18C9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8758DCFD-ACD4-4047-88E7-14852A69B746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="792" windowWidth="17280" windowHeight="9072" xr2:uid="{147A47B0-1836-4FF1-9A54-614DDF6AFE19}"/>
+    <workbookView xWindow="-9612" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{147A47B0-1836-4FF1-9A54-614DDF6AFE19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E072CA-4E92-41AA-9440-0406EC20240D}">
   <dimension ref="A2:M226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="B194" workbookViewId="0">
+      <selection activeCell="G210" sqref="G210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,14 +487,14 @@
       </c>
       <c r="C3">
         <f>SUM(I3:M3)</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="D3">
-        <v>44665</v>
+        <v>47775</v>
       </c>
       <c r="I3">
         <f>D3/7</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="J3">
         <f>E3/7</f>
@@ -519,11 +519,11 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C67" si="0">SUM(I4:M4)</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="I4">
         <f>D3/7</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="J4">
         <f>E3/7</f>
@@ -548,11 +548,11 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="I5">
         <f>D3/7</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="J5">
         <f>E3/7</f>
@@ -577,11 +577,11 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="I6">
         <f>D3/7</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="J6">
         <f>E3/7</f>
@@ -606,11 +606,11 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="I7">
         <f>D3/7</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="J7">
         <f>E3/7</f>
@@ -635,11 +635,11 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="I8">
         <f>D3/7</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="J8">
         <f>E3/7</f>
@@ -664,11 +664,11 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="I9">
         <f>D3/7</f>
-        <v>6380.7142857142853</v>
+        <v>6825</v>
       </c>
       <c r="J9">
         <f>E3/7</f>
@@ -705,23 +705,23 @@
         <v>4800</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I23" si="1">D10/7</f>
+        <f t="shared" ref="I10" si="1">D10/7</f>
         <v>9694.2857142857138</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J10:J23" si="2">E10/7</f>
+        <f t="shared" ref="J10" si="2">E10/7</f>
         <v>685.71428571428567</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K23" si="3">F10/7</f>
+        <f t="shared" ref="K10" si="3">F10/7</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L23" si="4">G10/7</f>
+        <f t="shared" ref="L10" si="4">G10/7</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:M23" si="5">H10/7</f>
+        <f t="shared" ref="M10" si="5">H10/7</f>
         <v>0</v>
       </c>
     </row>
@@ -734,23 +734,23 @@
         <v>10380</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I23" si="6">D10/7</f>
+        <f t="shared" ref="I11" si="6">D10/7</f>
         <v>9694.2857142857138</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11:J23" si="7">E10/7</f>
+        <f t="shared" ref="J11" si="7">E10/7</f>
         <v>685.71428571428567</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:K23" si="8">F10/7</f>
+        <f t="shared" ref="K11" si="8">F10/7</f>
         <v>0</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L23" si="9">G10/7</f>
+        <f t="shared" ref="L11" si="9">G10/7</f>
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:M23" si="10">H10/7</f>
+        <f t="shared" ref="M11" si="10">H10/7</f>
         <v>0</v>
       </c>
     </row>
@@ -914,23 +914,23 @@
         <v>32760</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:I23" si="16">D17/7</f>
+        <f t="shared" ref="I17" si="16">D17/7</f>
         <v>4680</v>
       </c>
       <c r="J17">
-        <f t="shared" ref="J17:J23" si="17">E17/7</f>
+        <f t="shared" ref="J17" si="17">E17/7</f>
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:K23" si="18">F17/7</f>
+        <f t="shared" ref="K17" si="18">F17/7</f>
         <v>0</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L23" si="19">G17/7</f>
+        <f t="shared" ref="L17" si="19">G17/7</f>
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17:M23" si="20">H17/7</f>
+        <f t="shared" ref="M17" si="20">H17/7</f>
         <v>0</v>
       </c>
     </row>
@@ -943,23 +943,23 @@
         <v>4680</v>
       </c>
       <c r="I18">
-        <f t="shared" ref="I18:I23" si="21">D17/7</f>
+        <f t="shared" ref="I18" si="21">D17/7</f>
         <v>4680</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:J23" si="22">E17/7</f>
+        <f t="shared" ref="J18" si="22">E17/7</f>
         <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:K23" si="23">F17/7</f>
+        <f t="shared" ref="K18" si="23">F17/7</f>
         <v>0</v>
       </c>
       <c r="L18">
-        <f t="shared" ref="L18:L23" si="24">G17/7</f>
+        <f t="shared" ref="L18" si="24">G17/7</f>
         <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" ref="M18:M23" si="25">H17/7</f>
+        <f t="shared" ref="M18" si="25">H17/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1123,23 +1123,23 @@
         <v>73710</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I55" si="31">D24/7</f>
+        <f t="shared" ref="I24" si="31">D24/7</f>
         <v>10530</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24:J55" si="32">E24/7</f>
+        <f t="shared" ref="J24" si="32">E24/7</f>
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" ref="K24:K55" si="33">F24/7</f>
+        <f t="shared" ref="K24" si="33">F24/7</f>
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:L55" si="34">G24/7</f>
+        <f t="shared" ref="L24" si="34">G24/7</f>
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:M55" si="35">H24/7</f>
+        <f t="shared" ref="M24" si="35">H24/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1152,23 +1152,23 @@
         <v>10530</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I56" si="36">D24/7</f>
+        <f t="shared" ref="I25" si="36">D24/7</f>
         <v>10530</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J56" si="37">E24/7</f>
+        <f t="shared" ref="J25" si="37">E24/7</f>
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K56" si="38">F24/7</f>
+        <f t="shared" ref="K25" si="38">F24/7</f>
         <v>0</v>
       </c>
       <c r="L25">
-        <f t="shared" ref="L25:L56" si="39">G24/7</f>
+        <f t="shared" ref="L25" si="39">G24/7</f>
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:M56" si="40">H24/7</f>
+        <f t="shared" ref="M25" si="40">H24/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1338,23 +1338,23 @@
         <v>24000</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I86" si="46">D31/7</f>
+        <f t="shared" ref="I31" si="46">D31/7</f>
         <v>7688.5714285714284</v>
       </c>
       <c r="J31">
-        <f t="shared" ref="J31:J86" si="47">E31/7</f>
+        <f t="shared" ref="J31" si="47">E31/7</f>
         <v>2742.8571428571427</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31:K86" si="48">F31/7</f>
+        <f t="shared" ref="K31" si="48">F31/7</f>
         <v>3428.5714285714284</v>
       </c>
       <c r="L31">
-        <f t="shared" ref="L31:L86" si="49">G31/7</f>
+        <f t="shared" ref="L31" si="49">G31/7</f>
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" ref="M31:M86" si="50">H31/7</f>
+        <f t="shared" ref="M31" si="50">H31/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1367,23 +1367,23 @@
         <v>13860</v>
       </c>
       <c r="I32">
-        <f t="shared" ref="I32:I86" si="51">D31/7</f>
+        <f t="shared" ref="I32" si="51">D31/7</f>
         <v>7688.5714285714284</v>
       </c>
       <c r="J32">
-        <f t="shared" ref="J32:J86" si="52">E31/7</f>
+        <f t="shared" ref="J32" si="52">E31/7</f>
         <v>2742.8571428571427</v>
       </c>
       <c r="K32">
-        <f t="shared" ref="K32:K86" si="53">F31/7</f>
+        <f t="shared" ref="K32" si="53">F31/7</f>
         <v>3428.5714285714284</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32:L86" si="54">G31/7</f>
+        <f t="shared" ref="L32" si="54">G31/7</f>
         <v>0</v>
       </c>
       <c r="M32">
-        <f t="shared" ref="M32:M86" si="55">H31/7</f>
+        <f t="shared" ref="M32" si="55">H31/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1550,23 +1550,23 @@
         <v>26400</v>
       </c>
       <c r="I38">
-        <f t="shared" ref="I38:I86" si="81">D38/7</f>
+        <f t="shared" ref="I38" si="81">D38/7</f>
         <v>8022.8571428571431</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J38:J86" si="82">E38/7</f>
+        <f t="shared" ref="J38" si="82">E38/7</f>
         <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" ref="K38:K86" si="83">F38/7</f>
+        <f t="shared" ref="K38" si="83">F38/7</f>
         <v>3771.4285714285716</v>
       </c>
       <c r="L38">
-        <f t="shared" ref="L38:L86" si="84">G38/7</f>
+        <f t="shared" ref="L38" si="84">G38/7</f>
         <v>0</v>
       </c>
       <c r="M38">
-        <f t="shared" ref="M38:M86" si="85">H38/7</f>
+        <f t="shared" ref="M38" si="85">H38/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1579,23 +1579,23 @@
         <v>11794.285714285714</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:I86" si="86">D38/7</f>
+        <f t="shared" ref="I39" si="86">D38/7</f>
         <v>8022.8571428571431</v>
       </c>
       <c r="J39">
-        <f t="shared" ref="J39:J86" si="87">E38/7</f>
+        <f t="shared" ref="J39" si="87">E38/7</f>
         <v>0</v>
       </c>
       <c r="K39">
-        <f t="shared" ref="K39:K86" si="88">F38/7</f>
+        <f t="shared" ref="K39" si="88">F38/7</f>
         <v>3771.4285714285716</v>
       </c>
       <c r="L39">
-        <f t="shared" ref="L39:L86" si="89">G38/7</f>
+        <f t="shared" ref="L39" si="89">G38/7</f>
         <v>0</v>
       </c>
       <c r="M39">
-        <f t="shared" ref="M39:M86" si="90">H38/7</f>
+        <f t="shared" ref="M39" si="90">H38/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1762,23 +1762,23 @@
         <v>50400</v>
       </c>
       <c r="I45">
-        <f t="shared" ref="I45:I86" si="116">D45/7</f>
+        <f t="shared" ref="I45" si="116">D45/7</f>
         <v>9694.2857142857138</v>
       </c>
       <c r="J45">
-        <f t="shared" ref="J45:J86" si="117">E45/7</f>
+        <f t="shared" ref="J45" si="117">E45/7</f>
         <v>0</v>
       </c>
       <c r="K45">
-        <f t="shared" ref="K45:K86" si="118">F45/7</f>
+        <f t="shared" ref="K45" si="118">F45/7</f>
         <v>7200</v>
       </c>
       <c r="L45">
-        <f t="shared" ref="L45:L86" si="119">G45/7</f>
+        <f t="shared" ref="L45" si="119">G45/7</f>
         <v>0</v>
       </c>
       <c r="M45">
-        <f t="shared" ref="M45:M86" si="120">H45/7</f>
+        <f t="shared" ref="M45" si="120">H45/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1791,23 +1791,23 @@
         <v>16894.285714285714</v>
       </c>
       <c r="I46">
-        <f t="shared" ref="I46:I86" si="121">D45/7</f>
+        <f t="shared" ref="I46" si="121">D45/7</f>
         <v>9694.2857142857138</v>
       </c>
       <c r="J46">
-        <f t="shared" ref="J46:J86" si="122">E45/7</f>
+        <f t="shared" ref="J46" si="122">E45/7</f>
         <v>0</v>
       </c>
       <c r="K46">
-        <f t="shared" ref="K46:K86" si="123">F45/7</f>
+        <f t="shared" ref="K46" si="123">F45/7</f>
         <v>7200</v>
       </c>
       <c r="L46">
-        <f t="shared" ref="L46:L86" si="124">G45/7</f>
+        <f t="shared" ref="L46" si="124">G45/7</f>
         <v>0</v>
       </c>
       <c r="M46">
-        <f t="shared" ref="M46:M86" si="125">H45/7</f>
+        <f t="shared" ref="M46" si="125">H45/7</f>
         <v>0</v>
       </c>
     </row>
@@ -1974,23 +1974,23 @@
         <v>24000</v>
       </c>
       <c r="I52">
-        <f t="shared" ref="I52:I86" si="131">D52/7</f>
+        <f t="shared" ref="I52" si="131">D52/7</f>
         <v>10028.571428571429</v>
       </c>
       <c r="J52">
-        <f t="shared" ref="J52:J86" si="132">E52/7</f>
+        <f t="shared" ref="J52" si="132">E52/7</f>
         <v>3428.5714285714284</v>
       </c>
       <c r="K52">
-        <f t="shared" ref="K52:K86" si="133">F52/7</f>
+        <f t="shared" ref="K52" si="133">F52/7</f>
         <v>0</v>
       </c>
       <c r="L52">
-        <f t="shared" ref="L52:L86" si="134">G52/7</f>
+        <f t="shared" ref="L52" si="134">G52/7</f>
         <v>0</v>
       </c>
       <c r="M52">
-        <f t="shared" ref="M52:M86" si="135">H52/7</f>
+        <f t="shared" ref="M52" si="135">H52/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2003,23 +2003,23 @@
         <v>13457.142857142859</v>
       </c>
       <c r="I53">
-        <f t="shared" ref="I53:I86" si="136">D52/7</f>
+        <f t="shared" ref="I53" si="136">D52/7</f>
         <v>10028.571428571429</v>
       </c>
       <c r="J53">
-        <f t="shared" ref="J53:J86" si="137">E52/7</f>
+        <f t="shared" ref="J53" si="137">E52/7</f>
         <v>3428.5714285714284</v>
       </c>
       <c r="K53">
-        <f t="shared" ref="K53:K86" si="138">F52/7</f>
+        <f t="shared" ref="K53" si="138">F52/7</f>
         <v>0</v>
       </c>
       <c r="L53">
-        <f t="shared" ref="L53:L86" si="139">G52/7</f>
+        <f t="shared" ref="L53" si="139">G52/7</f>
         <v>0</v>
       </c>
       <c r="M53">
-        <f t="shared" ref="M53:M86" si="140">H52/7</f>
+        <f t="shared" ref="M53" si="140">H52/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2189,23 +2189,23 @@
         <v>45600</v>
       </c>
       <c r="I59">
-        <f t="shared" ref="I59:I86" si="166">D59/7</f>
+        <f t="shared" ref="I59" si="166">D59/7</f>
         <v>11532.857142857143</v>
       </c>
       <c r="J59">
-        <f t="shared" ref="J59:J86" si="167">E59/7</f>
+        <f t="shared" ref="J59" si="167">E59/7</f>
         <v>4628.5714285714284</v>
       </c>
       <c r="K59">
-        <f t="shared" ref="K59:K86" si="168">F59/7</f>
+        <f t="shared" ref="K59" si="168">F59/7</f>
         <v>6514.2857142857147</v>
       </c>
       <c r="L59">
-        <f t="shared" ref="L59:L86" si="169">G59/7</f>
+        <f t="shared" ref="L59" si="169">G59/7</f>
         <v>0</v>
       </c>
       <c r="M59">
-        <f t="shared" ref="M59:M86" si="170">H59/7</f>
+        <f t="shared" ref="M59" si="170">H59/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2218,23 +2218,23 @@
         <v>22675.714285714286</v>
       </c>
       <c r="I60">
-        <f t="shared" ref="I60:I86" si="171">D59/7</f>
+        <f t="shared" ref="I60" si="171">D59/7</f>
         <v>11532.857142857143</v>
       </c>
       <c r="J60">
-        <f t="shared" ref="J60:J86" si="172">E59/7</f>
+        <f t="shared" ref="J60" si="172">E59/7</f>
         <v>4628.5714285714284</v>
       </c>
       <c r="K60">
-        <f t="shared" ref="K60:K86" si="173">F59/7</f>
+        <f t="shared" ref="K60" si="173">F59/7</f>
         <v>6514.2857142857147</v>
       </c>
       <c r="L60">
-        <f t="shared" ref="L60:L86" si="174">G59/7</f>
+        <f t="shared" ref="L60" si="174">G59/7</f>
         <v>0</v>
       </c>
       <c r="M60">
-        <f t="shared" ref="M60:M86" si="175">H59/7</f>
+        <f t="shared" ref="M60" si="175">H59/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2401,23 +2401,23 @@
         <v>93600</v>
       </c>
       <c r="I66">
-        <f t="shared" ref="I66:I86" si="201">D66/7</f>
+        <f t="shared" ref="I66" si="201">D66/7</f>
         <v>12535.714285714286</v>
       </c>
       <c r="J66">
-        <f t="shared" ref="J66:J86" si="202">E66/7</f>
+        <f t="shared" ref="J66" si="202">E66/7</f>
         <v>0</v>
       </c>
       <c r="K66">
-        <f t="shared" ref="K66:K86" si="203">F66/7</f>
+        <f t="shared" ref="K66" si="203">F66/7</f>
         <v>13371.428571428571</v>
       </c>
       <c r="L66">
-        <f t="shared" ref="L66:L86" si="204">G66/7</f>
+        <f t="shared" ref="L66" si="204">G66/7</f>
         <v>0</v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M86" si="205">H66/7</f>
+        <f t="shared" ref="M66" si="205">H66/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2430,23 +2430,23 @@
         <v>25907.142857142855</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I86" si="206">D66/7</f>
+        <f t="shared" ref="I67" si="206">D66/7</f>
         <v>12535.714285714286</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J86" si="207">E66/7</f>
+        <f t="shared" ref="J67" si="207">E66/7</f>
         <v>0</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K86" si="208">F66/7</f>
+        <f t="shared" ref="K67" si="208">F66/7</f>
         <v>13371.428571428571</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L86" si="209">G66/7</f>
+        <f t="shared" ref="L67" si="209">G66/7</f>
         <v>0</v>
       </c>
       <c r="M67">
-        <f t="shared" ref="M67:M86" si="210">H66/7</f>
+        <f t="shared" ref="M67" si="210">H66/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2604,32 +2604,29 @@
       </c>
       <c r="C73">
         <f t="shared" si="211"/>
-        <v>14592.857142857143</v>
+        <v>12535.714285714286</v>
       </c>
       <c r="D73">
         <v>87750</v>
       </c>
-      <c r="F73">
-        <v>14400</v>
-      </c>
       <c r="I73">
-        <f t="shared" ref="I73:I86" si="217">D73/7</f>
+        <f t="shared" ref="I73" si="217">D73/7</f>
         <v>12535.714285714286</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J86" si="218">E73/7</f>
+        <f t="shared" ref="J73" si="218">E73/7</f>
         <v>0</v>
       </c>
       <c r="K73">
-        <f t="shared" ref="K73:K86" si="219">F73/7</f>
-        <v>2057.1428571428573</v>
+        <f t="shared" ref="K73" si="219">F73/7</f>
+        <v>0</v>
       </c>
       <c r="L73">
-        <f t="shared" ref="L73:L86" si="220">G73/7</f>
+        <f t="shared" ref="L73" si="220">G73/7</f>
         <v>0</v>
       </c>
       <c r="M73">
-        <f t="shared" ref="M73:M86" si="221">H73/7</f>
+        <f t="shared" ref="M73" si="221">H73/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2639,26 +2636,26 @@
       </c>
       <c r="C74">
         <f t="shared" si="211"/>
-        <v>14592.857142857143</v>
+        <v>12535.714285714286</v>
       </c>
       <c r="I74">
-        <f t="shared" ref="I74:I86" si="222">D73/7</f>
+        <f t="shared" ref="I74" si="222">D73/7</f>
         <v>12535.714285714286</v>
       </c>
       <c r="J74">
-        <f t="shared" ref="J74:J86" si="223">E73/7</f>
+        <f t="shared" ref="J74" si="223">E73/7</f>
         <v>0</v>
       </c>
       <c r="K74">
-        <f t="shared" ref="K74:K86" si="224">F73/7</f>
-        <v>2057.1428571428573</v>
+        <f t="shared" ref="K74" si="224">F73/7</f>
+        <v>0</v>
       </c>
       <c r="L74">
-        <f t="shared" ref="L74:L86" si="225">G73/7</f>
+        <f t="shared" ref="L74" si="225">G73/7</f>
         <v>0</v>
       </c>
       <c r="M74">
-        <f t="shared" ref="M74:M86" si="226">H73/7</f>
+        <f t="shared" ref="M74" si="226">H73/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2668,7 +2665,7 @@
       </c>
       <c r="C75">
         <f t="shared" si="211"/>
-        <v>14592.857142857143</v>
+        <v>12535.714285714286</v>
       </c>
       <c r="I75">
         <f t="shared" ref="I75" si="227">D73/7</f>
@@ -2680,7 +2677,7 @@
       </c>
       <c r="K75">
         <f t="shared" ref="K75" si="229">F73/7</f>
-        <v>2057.1428571428573</v>
+        <v>0</v>
       </c>
       <c r="L75">
         <f t="shared" ref="L75" si="230">G73/7</f>
@@ -2697,7 +2694,7 @@
       </c>
       <c r="C76">
         <f t="shared" si="211"/>
-        <v>14592.857142857143</v>
+        <v>12535.714285714286</v>
       </c>
       <c r="I76">
         <f t="shared" ref="I76" si="232">D73/7</f>
@@ -2709,7 +2706,7 @@
       </c>
       <c r="K76">
         <f t="shared" ref="K76" si="234">F73/7</f>
-        <v>2057.1428571428573</v>
+        <v>0</v>
       </c>
       <c r="L76">
         <f t="shared" ref="L76" si="235">G73/7</f>
@@ -2726,7 +2723,7 @@
       </c>
       <c r="C77">
         <f t="shared" si="211"/>
-        <v>14592.857142857143</v>
+        <v>12535.714285714286</v>
       </c>
       <c r="I77">
         <f t="shared" ref="I77" si="237">D73/7</f>
@@ -2738,7 +2735,7 @@
       </c>
       <c r="K77">
         <f t="shared" ref="K77" si="239">F73/7</f>
-        <v>2057.1428571428573</v>
+        <v>0</v>
       </c>
       <c r="L77">
         <f t="shared" ref="L77" si="240">G73/7</f>
@@ -2755,7 +2752,7 @@
       </c>
       <c r="C78">
         <f t="shared" si="211"/>
-        <v>14592.857142857143</v>
+        <v>12535.714285714286</v>
       </c>
       <c r="I78">
         <f t="shared" ref="I78" si="242">D73/7</f>
@@ -2767,7 +2764,7 @@
       </c>
       <c r="K78">
         <f t="shared" ref="K78" si="244">F73/7</f>
-        <v>2057.1428571428573</v>
+        <v>0</v>
       </c>
       <c r="L78">
         <f t="shared" ref="L78" si="245">G73/7</f>
@@ -2784,7 +2781,7 @@
       </c>
       <c r="C79">
         <f t="shared" si="211"/>
-        <v>14592.857142857143</v>
+        <v>12535.714285714286</v>
       </c>
       <c r="I79">
         <f t="shared" ref="I79" si="247">D73/7</f>
@@ -2796,7 +2793,7 @@
       </c>
       <c r="K79">
         <f t="shared" ref="K79" si="249">F73/7</f>
-        <v>2057.1428571428573</v>
+        <v>0</v>
       </c>
       <c r="L79">
         <f t="shared" ref="L79" si="250">G73/7</f>
@@ -2816,7 +2813,7 @@
       </c>
       <c r="C80">
         <f t="shared" si="211"/>
-        <v>24444.857142857141</v>
+        <v>22568.571428571428</v>
       </c>
       <c r="D80">
         <v>109980</v>
@@ -2824,27 +2821,24 @@
       <c r="E80">
         <v>48000</v>
       </c>
-      <c r="F80">
-        <v>13134</v>
-      </c>
       <c r="I80">
-        <f t="shared" ref="I80:I86" si="252">D80/7</f>
+        <f t="shared" ref="I80" si="252">D80/7</f>
         <v>15711.428571428571</v>
       </c>
       <c r="J80">
-        <f t="shared" ref="J80:J86" si="253">E80/7</f>
+        <f t="shared" ref="J80" si="253">E80/7</f>
         <v>6857.1428571428569</v>
       </c>
       <c r="K80">
-        <f t="shared" ref="K80:K86" si="254">F80/7</f>
-        <v>1876.2857142857142</v>
+        <f t="shared" ref="K80" si="254">F80/7</f>
+        <v>0</v>
       </c>
       <c r="L80">
-        <f t="shared" ref="L80:L86" si="255">G80/7</f>
+        <f t="shared" ref="L80" si="255">G80/7</f>
         <v>0</v>
       </c>
       <c r="M80">
-        <f t="shared" ref="M80:M86" si="256">H80/7</f>
+        <f t="shared" ref="M80" si="256">H80/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2854,26 +2848,26 @@
       </c>
       <c r="C81">
         <f t="shared" si="211"/>
-        <v>24444.857142857141</v>
+        <v>22568.571428571428</v>
       </c>
       <c r="I81">
-        <f t="shared" ref="I81:I86" si="257">D80/7</f>
+        <f t="shared" ref="I81" si="257">D80/7</f>
         <v>15711.428571428571</v>
       </c>
       <c r="J81">
-        <f t="shared" ref="J81:J86" si="258">E80/7</f>
+        <f t="shared" ref="J81" si="258">E80/7</f>
         <v>6857.1428571428569</v>
       </c>
       <c r="K81">
-        <f t="shared" ref="K81:K86" si="259">F80/7</f>
-        <v>1876.2857142857142</v>
+        <f t="shared" ref="K81" si="259">F80/7</f>
+        <v>0</v>
       </c>
       <c r="L81">
-        <f t="shared" ref="L81:L86" si="260">G80/7</f>
+        <f t="shared" ref="L81" si="260">G80/7</f>
         <v>0</v>
       </c>
       <c r="M81">
-        <f t="shared" ref="M81:M86" si="261">H80/7</f>
+        <f t="shared" ref="M81" si="261">H80/7</f>
         <v>0</v>
       </c>
     </row>
@@ -2883,7 +2877,7 @@
       </c>
       <c r="C82">
         <f t="shared" si="211"/>
-        <v>24444.857142857141</v>
+        <v>22568.571428571428</v>
       </c>
       <c r="I82">
         <f t="shared" ref="I82" si="262">D80/7</f>
@@ -2895,7 +2889,7 @@
       </c>
       <c r="K82">
         <f t="shared" ref="K82" si="264">F80/7</f>
-        <v>1876.2857142857142</v>
+        <v>0</v>
       </c>
       <c r="L82">
         <f t="shared" ref="L82" si="265">G80/7</f>
@@ -2912,7 +2906,7 @@
       </c>
       <c r="C83">
         <f t="shared" si="211"/>
-        <v>24444.857142857141</v>
+        <v>22568.571428571428</v>
       </c>
       <c r="I83">
         <f t="shared" ref="I83" si="267">D80/7</f>
@@ -2924,7 +2918,7 @@
       </c>
       <c r="K83">
         <f t="shared" ref="K83" si="269">F80/7</f>
-        <v>1876.2857142857142</v>
+        <v>0</v>
       </c>
       <c r="L83">
         <f t="shared" ref="L83" si="270">G80/7</f>
@@ -2941,7 +2935,7 @@
       </c>
       <c r="C84">
         <f t="shared" si="211"/>
-        <v>24444.857142857141</v>
+        <v>22568.571428571428</v>
       </c>
       <c r="I84">
         <f t="shared" ref="I84" si="272">D80/7</f>
@@ -2953,7 +2947,7 @@
       </c>
       <c r="K84">
         <f t="shared" ref="K84" si="274">F80/7</f>
-        <v>1876.2857142857142</v>
+        <v>0</v>
       </c>
       <c r="L84">
         <f t="shared" ref="L84" si="275">G80/7</f>
@@ -2970,7 +2964,7 @@
       </c>
       <c r="C85">
         <f t="shared" si="211"/>
-        <v>24444.857142857141</v>
+        <v>22568.571428571428</v>
       </c>
       <c r="I85">
         <f t="shared" ref="I85" si="277">D80/7</f>
@@ -2982,7 +2976,7 @@
       </c>
       <c r="K85">
         <f t="shared" ref="K85" si="279">F80/7</f>
-        <v>1876.2857142857142</v>
+        <v>0</v>
       </c>
       <c r="L85">
         <f t="shared" ref="L85" si="280">G80/7</f>
@@ -2999,7 +2993,7 @@
       </c>
       <c r="C86">
         <f t="shared" si="211"/>
-        <v>24444.857142857141</v>
+        <v>22568.571428571428</v>
       </c>
       <c r="I86">
         <f t="shared" ref="I86" si="282">D80/7</f>
@@ -3011,7 +3005,7 @@
       </c>
       <c r="K86">
         <f t="shared" ref="K86" si="284">F80/7</f>
-        <v>1876.2857142857142</v>
+        <v>0</v>
       </c>
       <c r="L86">
         <f t="shared" ref="L86" si="285">G80/7</f>
@@ -3031,13 +3025,10 @@
       </c>
       <c r="C87">
         <f t="shared" si="211"/>
-        <v>34599.428571428572</v>
+        <v>16045.714285714286</v>
       </c>
       <c r="D87">
         <v>112320</v>
-      </c>
-      <c r="F87">
-        <v>129876</v>
       </c>
       <c r="I87">
         <f>D87/7</f>
@@ -3049,7 +3040,7 @@
       </c>
       <c r="K87">
         <f>F87/7</f>
-        <v>18553.714285714286</v>
+        <v>0</v>
       </c>
       <c r="L87">
         <f>G87/7</f>
@@ -3066,7 +3057,7 @@
       </c>
       <c r="C88">
         <f t="shared" si="211"/>
-        <v>34599.428571428572</v>
+        <v>16045.714285714286</v>
       </c>
       <c r="I88">
         <f>D87/7</f>
@@ -3078,7 +3069,7 @@
       </c>
       <c r="K88">
         <f>F87/7</f>
-        <v>18553.714285714286</v>
+        <v>0</v>
       </c>
       <c r="L88">
         <f>G87/7</f>
@@ -3095,7 +3086,7 @@
       </c>
       <c r="C89">
         <f t="shared" si="211"/>
-        <v>34599.428571428572</v>
+        <v>16045.714285714286</v>
       </c>
       <c r="I89">
         <f>D87/7</f>
@@ -3107,7 +3098,7 @@
       </c>
       <c r="K89">
         <f>F87/7</f>
-        <v>18553.714285714286</v>
+        <v>0</v>
       </c>
       <c r="L89">
         <f>G87/7</f>
@@ -3124,7 +3115,7 @@
       </c>
       <c r="C90">
         <f t="shared" si="211"/>
-        <v>34599.428571428572</v>
+        <v>16045.714285714286</v>
       </c>
       <c r="I90">
         <f>D87/7</f>
@@ -3136,7 +3127,7 @@
       </c>
       <c r="K90">
         <f>F87/7</f>
-        <v>18553.714285714286</v>
+        <v>0</v>
       </c>
       <c r="L90">
         <f>G87/7</f>
@@ -3153,7 +3144,7 @@
       </c>
       <c r="C91">
         <f t="shared" si="211"/>
-        <v>34599.428571428572</v>
+        <v>16045.714285714286</v>
       </c>
       <c r="I91">
         <f>D87/7</f>
@@ -3165,7 +3156,7 @@
       </c>
       <c r="K91">
         <f>F87/7</f>
-        <v>18553.714285714286</v>
+        <v>0</v>
       </c>
       <c r="L91">
         <f>G87/7</f>
@@ -3182,7 +3173,7 @@
       </c>
       <c r="C92">
         <f t="shared" si="211"/>
-        <v>34599.428571428572</v>
+        <v>16045.714285714286</v>
       </c>
       <c r="I92">
         <f>D87/7</f>
@@ -3194,7 +3185,7 @@
       </c>
       <c r="K92">
         <f>F87/7</f>
-        <v>18553.714285714286</v>
+        <v>0</v>
       </c>
       <c r="L92">
         <f>G87/7</f>
@@ -3211,7 +3202,7 @@
       </c>
       <c r="C93">
         <f t="shared" si="211"/>
-        <v>34599.428571428572</v>
+        <v>16045.714285714286</v>
       </c>
       <c r="I93">
         <f>D87/7</f>
@@ -3223,7 +3214,7 @@
       </c>
       <c r="K93">
         <f>F87/7</f>
-        <v>18553.714285714286</v>
+        <v>0</v>
       </c>
       <c r="L93">
         <f>G87/7</f>
@@ -3243,35 +3234,33 @@
       </c>
       <c r="C94">
         <f t="shared" si="211"/>
-        <v>38156.142857142862</v>
+        <v>35078.571428571428</v>
       </c>
       <c r="D94">
-        <v>202410</v>
+        <v>204750</v>
       </c>
       <c r="E94">
-        <v>31200</v>
-      </c>
-      <c r="F94" s="2">
-        <v>33483</v>
-      </c>
+        <v>40800</v>
+      </c>
+      <c r="F94" s="2"/>
       <c r="I94">
-        <f t="shared" ref="I94:I125" si="287">D94/7</f>
-        <v>28915.714285714286</v>
+        <f t="shared" ref="I94" si="287">D94/7</f>
+        <v>29250</v>
       </c>
       <c r="J94">
-        <f t="shared" ref="J94:J125" si="288">E94/7</f>
-        <v>4457.1428571428569</v>
+        <f t="shared" ref="J94" si="288">E94/7</f>
+        <v>5828.5714285714284</v>
       </c>
       <c r="K94">
-        <f t="shared" ref="K94:K125" si="289">F94/7</f>
-        <v>4783.2857142857147</v>
+        <f t="shared" ref="K94" si="289">F94/7</f>
+        <v>0</v>
       </c>
       <c r="L94">
-        <f t="shared" ref="L94:L125" si="290">G94/7</f>
+        <f t="shared" ref="L94" si="290">G94/7</f>
         <v>0</v>
       </c>
       <c r="M94">
-        <f t="shared" ref="M94:M125" si="291">H94/7</f>
+        <f t="shared" ref="M94" si="291">H94/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3281,26 +3270,26 @@
       </c>
       <c r="C95">
         <f t="shared" si="211"/>
-        <v>38156.142857142862</v>
+        <v>35078.571428571428</v>
       </c>
       <c r="I95">
-        <f t="shared" ref="I95:I126" si="292">D94/7</f>
-        <v>28915.714285714286</v>
+        <f t="shared" ref="I95" si="292">D94/7</f>
+        <v>29250</v>
       </c>
       <c r="J95">
-        <f t="shared" ref="J95:J126" si="293">E94/7</f>
-        <v>4457.1428571428569</v>
+        <f t="shared" ref="J95" si="293">E94/7</f>
+        <v>5828.5714285714284</v>
       </c>
       <c r="K95">
-        <f t="shared" ref="K95:K126" si="294">F94/7</f>
-        <v>4783.2857142857147</v>
+        <f t="shared" ref="K95" si="294">F94/7</f>
+        <v>0</v>
       </c>
       <c r="L95">
-        <f t="shared" ref="L95:L126" si="295">G94/7</f>
+        <f t="shared" ref="L95" si="295">G94/7</f>
         <v>0</v>
       </c>
       <c r="M95">
-        <f t="shared" ref="M95:M126" si="296">H94/7</f>
+        <f t="shared" ref="M95" si="296">H94/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3310,19 +3299,19 @@
       </c>
       <c r="C96">
         <f t="shared" si="211"/>
-        <v>38156.142857142862</v>
+        <v>35078.571428571428</v>
       </c>
       <c r="I96">
         <f t="shared" ref="I96:M96" si="297">D94/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J96">
         <f t="shared" si="297"/>
-        <v>4457.1428571428569</v>
+        <v>5828.5714285714284</v>
       </c>
       <c r="K96">
         <f t="shared" si="297"/>
-        <v>4783.2857142857147</v>
+        <v>0</v>
       </c>
       <c r="L96">
         <f t="shared" si="297"/>
@@ -3339,19 +3328,19 @@
       </c>
       <c r="C97">
         <f t="shared" si="211"/>
-        <v>38156.142857142862</v>
+        <v>35078.571428571428</v>
       </c>
       <c r="I97">
         <f t="shared" ref="I97:M97" si="298">D94/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J97">
         <f t="shared" si="298"/>
-        <v>4457.1428571428569</v>
+        <v>5828.5714285714284</v>
       </c>
       <c r="K97">
         <f t="shared" si="298"/>
-        <v>4783.2857142857147</v>
+        <v>0</v>
       </c>
       <c r="L97">
         <f t="shared" si="298"/>
@@ -3368,19 +3357,19 @@
       </c>
       <c r="C98">
         <f t="shared" si="211"/>
-        <v>38156.142857142862</v>
+        <v>35078.571428571428</v>
       </c>
       <c r="I98">
         <f t="shared" ref="I98:M98" si="299">D94/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J98">
         <f t="shared" si="299"/>
-        <v>4457.1428571428569</v>
+        <v>5828.5714285714284</v>
       </c>
       <c r="K98">
         <f t="shared" si="299"/>
-        <v>4783.2857142857147</v>
+        <v>0</v>
       </c>
       <c r="L98">
         <f t="shared" si="299"/>
@@ -3397,19 +3386,19 @@
       </c>
       <c r="C99">
         <f t="shared" si="211"/>
-        <v>38156.142857142862</v>
+        <v>35078.571428571428</v>
       </c>
       <c r="I99">
         <f t="shared" ref="I99:M99" si="300">D94/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J99">
         <f t="shared" si="300"/>
-        <v>4457.1428571428569</v>
+        <v>5828.5714285714284</v>
       </c>
       <c r="K99">
         <f t="shared" si="300"/>
-        <v>4783.2857142857147</v>
+        <v>0</v>
       </c>
       <c r="L99">
         <f t="shared" si="300"/>
@@ -3426,19 +3415,19 @@
       </c>
       <c r="C100">
         <f t="shared" si="211"/>
-        <v>38156.142857142862</v>
+        <v>35078.571428571428</v>
       </c>
       <c r="I100">
         <f t="shared" ref="I100:M100" si="301">D94/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J100">
         <f t="shared" si="301"/>
-        <v>4457.1428571428569</v>
+        <v>5828.5714285714284</v>
       </c>
       <c r="K100">
         <f t="shared" si="301"/>
-        <v>4783.2857142857147</v>
+        <v>0</v>
       </c>
       <c r="L100">
         <f t="shared" si="301"/>
@@ -3458,32 +3447,29 @@
       </c>
       <c r="C101">
         <f t="shared" si="211"/>
-        <v>33411.71428571429</v>
+        <v>29250</v>
       </c>
       <c r="D101">
-        <v>202410</v>
-      </c>
-      <c r="F101">
-        <v>31472</v>
+        <v>204750</v>
       </c>
       <c r="I101">
-        <f t="shared" ref="I101:I132" si="302">D101/7</f>
-        <v>28915.714285714286</v>
+        <f t="shared" ref="I101" si="302">D101/7</f>
+        <v>29250</v>
       </c>
       <c r="J101">
-        <f t="shared" ref="J101:J132" si="303">E101/7</f>
+        <f t="shared" ref="J101" si="303">E101/7</f>
         <v>0</v>
       </c>
       <c r="K101">
-        <f t="shared" ref="K101:K132" si="304">F101/7</f>
-        <v>4496</v>
+        <f t="shared" ref="K101" si="304">F101/7</f>
+        <v>0</v>
       </c>
       <c r="L101">
-        <f t="shared" ref="L101:L132" si="305">G101/7</f>
+        <f t="shared" ref="L101" si="305">G101/7</f>
         <v>0</v>
       </c>
       <c r="M101">
-        <f t="shared" ref="M101:M132" si="306">H101/7</f>
+        <f t="shared" ref="M101" si="306">H101/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3493,26 +3479,26 @@
       </c>
       <c r="C102">
         <f t="shared" si="211"/>
-        <v>33411.71428571429</v>
+        <v>29250</v>
       </c>
       <c r="I102">
-        <f t="shared" ref="I102:I133" si="307">D101/7</f>
-        <v>28915.714285714286</v>
+        <f t="shared" ref="I102" si="307">D101/7</f>
+        <v>29250</v>
       </c>
       <c r="J102">
-        <f t="shared" ref="J102:J133" si="308">E101/7</f>
+        <f t="shared" ref="J102" si="308">E101/7</f>
         <v>0</v>
       </c>
       <c r="K102">
-        <f t="shared" ref="K102:K133" si="309">F101/7</f>
-        <v>4496</v>
+        <f t="shared" ref="K102" si="309">F101/7</f>
+        <v>0</v>
       </c>
       <c r="L102">
-        <f t="shared" ref="L102:L133" si="310">G101/7</f>
+        <f t="shared" ref="L102" si="310">G101/7</f>
         <v>0</v>
       </c>
       <c r="M102">
-        <f t="shared" ref="M102:M133" si="311">H101/7</f>
+        <f t="shared" ref="M102" si="311">H101/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3522,11 +3508,11 @@
       </c>
       <c r="C103">
         <f t="shared" si="211"/>
-        <v>33411.71428571429</v>
+        <v>29250</v>
       </c>
       <c r="I103">
         <f t="shared" ref="I103:M103" si="312">D101/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J103">
         <f t="shared" si="312"/>
@@ -3534,7 +3520,7 @@
       </c>
       <c r="K103">
         <f t="shared" si="312"/>
-        <v>4496</v>
+        <v>0</v>
       </c>
       <c r="L103">
         <f t="shared" si="312"/>
@@ -3551,11 +3537,11 @@
       </c>
       <c r="C104">
         <f t="shared" si="211"/>
-        <v>33411.71428571429</v>
+        <v>29250</v>
       </c>
       <c r="I104">
         <f t="shared" ref="I104:M104" si="313">D101/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J104">
         <f t="shared" si="313"/>
@@ -3563,7 +3549,7 @@
       </c>
       <c r="K104">
         <f t="shared" si="313"/>
-        <v>4496</v>
+        <v>0</v>
       </c>
       <c r="L104">
         <f t="shared" si="313"/>
@@ -3580,11 +3566,11 @@
       </c>
       <c r="C105">
         <f t="shared" si="211"/>
-        <v>33411.71428571429</v>
+        <v>29250</v>
       </c>
       <c r="I105">
         <f t="shared" ref="I105:M105" si="314">D101/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J105">
         <f t="shared" si="314"/>
@@ -3592,7 +3578,7 @@
       </c>
       <c r="K105">
         <f t="shared" si="314"/>
-        <v>4496</v>
+        <v>0</v>
       </c>
       <c r="L105">
         <f t="shared" si="314"/>
@@ -3609,11 +3595,11 @@
       </c>
       <c r="C106">
         <f t="shared" si="211"/>
-        <v>33411.71428571429</v>
+        <v>29250</v>
       </c>
       <c r="I106">
         <f t="shared" ref="I106:M106" si="315">D101/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J106">
         <f t="shared" si="315"/>
@@ -3621,7 +3607,7 @@
       </c>
       <c r="K106">
         <f t="shared" si="315"/>
-        <v>4496</v>
+        <v>0</v>
       </c>
       <c r="L106">
         <f t="shared" si="315"/>
@@ -3638,11 +3624,11 @@
       </c>
       <c r="C107">
         <f t="shared" si="211"/>
-        <v>33411.71428571429</v>
+        <v>29250</v>
       </c>
       <c r="I107">
         <f t="shared" ref="I107:M107" si="316">D101/7</f>
-        <v>28915.714285714286</v>
+        <v>29250</v>
       </c>
       <c r="J107">
         <f t="shared" si="316"/>
@@ -3650,7 +3636,7 @@
       </c>
       <c r="K107">
         <f t="shared" si="316"/>
-        <v>4496</v>
+        <v>0</v>
       </c>
       <c r="L107">
         <f t="shared" si="316"/>
@@ -3670,38 +3656,32 @@
       </c>
       <c r="C108">
         <f t="shared" si="211"/>
-        <v>48725.571428571428</v>
+        <v>35760</v>
       </c>
       <c r="D108">
-        <v>202410</v>
+        <v>205920</v>
       </c>
       <c r="E108">
         <v>44400</v>
       </c>
-      <c r="F108">
-        <v>52269</v>
-      </c>
-      <c r="G108">
-        <v>42000</v>
-      </c>
       <c r="I108">
-        <f t="shared" ref="I108:I139" si="317">D108/7</f>
-        <v>28915.714285714286</v>
+        <f t="shared" ref="I108" si="317">D108/7</f>
+        <v>29417.142857142859</v>
       </c>
       <c r="J108">
-        <f t="shared" ref="J108:J139" si="318">E108/7</f>
+        <f t="shared" ref="J108" si="318">E108/7</f>
         <v>6342.8571428571431</v>
       </c>
       <c r="K108">
-        <f t="shared" ref="K108:K139" si="319">F108/7</f>
-        <v>7467</v>
+        <f t="shared" ref="K108" si="319">F108/7</f>
+        <v>0</v>
       </c>
       <c r="L108">
-        <f t="shared" ref="L108:L139" si="320">G108/7</f>
-        <v>6000</v>
+        <f t="shared" ref="L108" si="320">G108/7</f>
+        <v>0</v>
       </c>
       <c r="M108">
-        <f t="shared" ref="M108:M139" si="321">H108/7</f>
+        <f t="shared" ref="M108" si="321">H108/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3711,26 +3691,26 @@
       </c>
       <c r="C109">
         <f t="shared" si="211"/>
-        <v>48725.571428571428</v>
+        <v>35760</v>
       </c>
       <c r="I109">
-        <f t="shared" ref="I109:I140" si="322">D108/7</f>
-        <v>28915.714285714286</v>
+        <f t="shared" ref="I109" si="322">D108/7</f>
+        <v>29417.142857142859</v>
       </c>
       <c r="J109">
-        <f t="shared" ref="J109:J140" si="323">E108/7</f>
+        <f t="shared" ref="J109" si="323">E108/7</f>
         <v>6342.8571428571431</v>
       </c>
       <c r="K109">
-        <f t="shared" ref="K109:K140" si="324">F108/7</f>
-        <v>7467</v>
+        <f t="shared" ref="K109" si="324">F108/7</f>
+        <v>0</v>
       </c>
       <c r="L109">
-        <f t="shared" ref="L109:L140" si="325">G108/7</f>
-        <v>6000</v>
+        <f t="shared" ref="L109" si="325">G108/7</f>
+        <v>0</v>
       </c>
       <c r="M109">
-        <f t="shared" ref="M109:M140" si="326">H108/7</f>
+        <f t="shared" ref="M109" si="326">H108/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3740,11 +3720,11 @@
       </c>
       <c r="C110">
         <f t="shared" si="211"/>
-        <v>48725.571428571428</v>
+        <v>35760</v>
       </c>
       <c r="I110">
         <f t="shared" ref="I110:M110" si="327">D108/7</f>
-        <v>28915.714285714286</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J110">
         <f t="shared" si="327"/>
@@ -3752,11 +3732,11 @@
       </c>
       <c r="K110">
         <f t="shared" si="327"/>
-        <v>7467</v>
+        <v>0</v>
       </c>
       <c r="L110">
         <f t="shared" si="327"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M110">
         <f t="shared" si="327"/>
@@ -3769,11 +3749,11 @@
       </c>
       <c r="C111">
         <f t="shared" si="211"/>
-        <v>48725.571428571428</v>
+        <v>35760</v>
       </c>
       <c r="I111">
         <f t="shared" ref="I111:M111" si="328">D108/7</f>
-        <v>28915.714285714286</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J111">
         <f t="shared" si="328"/>
@@ -3781,11 +3761,11 @@
       </c>
       <c r="K111">
         <f t="shared" si="328"/>
-        <v>7467</v>
+        <v>0</v>
       </c>
       <c r="L111">
         <f t="shared" si="328"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M111">
         <f t="shared" si="328"/>
@@ -3798,11 +3778,11 @@
       </c>
       <c r="C112">
         <f t="shared" si="211"/>
-        <v>48725.571428571428</v>
+        <v>35760</v>
       </c>
       <c r="I112">
         <f t="shared" ref="I112:M112" si="329">D108/7</f>
-        <v>28915.714285714286</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J112">
         <f t="shared" si="329"/>
@@ -3810,11 +3790,11 @@
       </c>
       <c r="K112">
         <f t="shared" si="329"/>
-        <v>7467</v>
+        <v>0</v>
       </c>
       <c r="L112">
         <f t="shared" si="329"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M112">
         <f t="shared" si="329"/>
@@ -3827,11 +3807,11 @@
       </c>
       <c r="C113">
         <f t="shared" si="211"/>
-        <v>48725.571428571428</v>
+        <v>35760</v>
       </c>
       <c r="I113">
         <f t="shared" ref="I113:M113" si="330">D108/7</f>
-        <v>28915.714285714286</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J113">
         <f t="shared" si="330"/>
@@ -3839,11 +3819,11 @@
       </c>
       <c r="K113">
         <f t="shared" si="330"/>
-        <v>7467</v>
+        <v>0</v>
       </c>
       <c r="L113">
         <f t="shared" si="330"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M113">
         <f t="shared" si="330"/>
@@ -3856,11 +3836,11 @@
       </c>
       <c r="C114">
         <f t="shared" si="211"/>
-        <v>48725.571428571428</v>
+        <v>35760</v>
       </c>
       <c r="I114">
         <f t="shared" ref="I114:M114" si="331">D108/7</f>
-        <v>28915.714285714286</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J114">
         <f t="shared" si="331"/>
@@ -3868,11 +3848,11 @@
       </c>
       <c r="K114">
         <f t="shared" si="331"/>
-        <v>7467</v>
+        <v>0</v>
       </c>
       <c r="L114">
         <f t="shared" si="331"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M114">
         <f t="shared" si="331"/>
@@ -3888,35 +3868,29 @@
       </c>
       <c r="C115">
         <f t="shared" si="211"/>
-        <v>56407</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="D115">
-        <v>203580</v>
-      </c>
-      <c r="F115">
-        <v>149269</v>
-      </c>
-      <c r="G115">
-        <v>42000</v>
+        <v>205920</v>
       </c>
       <c r="I115">
-        <f t="shared" ref="I115:I146" si="332">D115/7</f>
-        <v>29082.857142857141</v>
+        <f t="shared" ref="I115" si="332">D115/7</f>
+        <v>29417.142857142859</v>
       </c>
       <c r="J115">
-        <f t="shared" ref="J115:J146" si="333">E115/7</f>
+        <f t="shared" ref="J115" si="333">E115/7</f>
         <v>0</v>
       </c>
       <c r="K115">
-        <f t="shared" ref="K115:K146" si="334">F115/7</f>
-        <v>21324.142857142859</v>
+        <f t="shared" ref="K115" si="334">F115/7</f>
+        <v>0</v>
       </c>
       <c r="L115">
-        <f t="shared" ref="L115:L146" si="335">G115/7</f>
-        <v>6000</v>
+        <f t="shared" ref="L115" si="335">G115/7</f>
+        <v>0</v>
       </c>
       <c r="M115">
-        <f t="shared" ref="M115:M146" si="336">H115/7</f>
+        <f t="shared" ref="M115" si="336">H115/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3926,26 +3900,26 @@
       </c>
       <c r="C116">
         <f t="shared" si="211"/>
-        <v>56407</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="I116">
-        <f t="shared" ref="I116:I147" si="337">D115/7</f>
-        <v>29082.857142857141</v>
+        <f t="shared" ref="I116" si="337">D115/7</f>
+        <v>29417.142857142859</v>
       </c>
       <c r="J116">
-        <f t="shared" ref="J116:J147" si="338">E115/7</f>
+        <f t="shared" ref="J116" si="338">E115/7</f>
         <v>0</v>
       </c>
       <c r="K116">
-        <f t="shared" ref="K116:K147" si="339">F115/7</f>
-        <v>21324.142857142859</v>
+        <f t="shared" ref="K116" si="339">F115/7</f>
+        <v>0</v>
       </c>
       <c r="L116">
-        <f t="shared" ref="L116:L147" si="340">G115/7</f>
-        <v>6000</v>
+        <f t="shared" ref="L116" si="340">G115/7</f>
+        <v>0</v>
       </c>
       <c r="M116">
-        <f t="shared" ref="M116:M147" si="341">H115/7</f>
+        <f t="shared" ref="M116" si="341">H115/7</f>
         <v>0</v>
       </c>
     </row>
@@ -3955,11 +3929,11 @@
       </c>
       <c r="C117">
         <f t="shared" si="211"/>
-        <v>56407</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="I117">
         <f t="shared" ref="I117:M117" si="342">D115/7</f>
-        <v>29082.857142857141</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J117">
         <f t="shared" si="342"/>
@@ -3967,11 +3941,11 @@
       </c>
       <c r="K117">
         <f t="shared" si="342"/>
-        <v>21324.142857142859</v>
+        <v>0</v>
       </c>
       <c r="L117">
         <f t="shared" si="342"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M117">
         <f t="shared" si="342"/>
@@ -3984,11 +3958,11 @@
       </c>
       <c r="C118">
         <f t="shared" si="211"/>
-        <v>56407</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="I118">
         <f t="shared" ref="I118:M118" si="343">D115/7</f>
-        <v>29082.857142857141</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J118">
         <f t="shared" si="343"/>
@@ -3996,11 +3970,11 @@
       </c>
       <c r="K118">
         <f t="shared" si="343"/>
-        <v>21324.142857142859</v>
+        <v>0</v>
       </c>
       <c r="L118">
         <f t="shared" si="343"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M118">
         <f t="shared" si="343"/>
@@ -4013,11 +3987,11 @@
       </c>
       <c r="C119">
         <f t="shared" si="211"/>
-        <v>56407</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="I119">
         <f t="shared" ref="I119:M119" si="344">D115/7</f>
-        <v>29082.857142857141</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J119">
         <f t="shared" si="344"/>
@@ -4025,11 +3999,11 @@
       </c>
       <c r="K119">
         <f t="shared" si="344"/>
-        <v>21324.142857142859</v>
+        <v>0</v>
       </c>
       <c r="L119">
         <f t="shared" si="344"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M119">
         <f t="shared" si="344"/>
@@ -4042,11 +4016,11 @@
       </c>
       <c r="C120">
         <f t="shared" si="211"/>
-        <v>56407</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="I120">
         <f t="shared" ref="I120:M120" si="345">D115/7</f>
-        <v>29082.857142857141</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J120">
         <f t="shared" si="345"/>
@@ -4054,11 +4028,11 @@
       </c>
       <c r="K120">
         <f t="shared" si="345"/>
-        <v>21324.142857142859</v>
+        <v>0</v>
       </c>
       <c r="L120">
         <f t="shared" si="345"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M120">
         <f t="shared" si="345"/>
@@ -4071,11 +4045,11 @@
       </c>
       <c r="C121">
         <f t="shared" si="211"/>
-        <v>56407</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="I121">
         <f t="shared" ref="I121:M121" si="346">D115/7</f>
-        <v>29082.857142857141</v>
+        <v>29417.142857142859</v>
       </c>
       <c r="J121">
         <f t="shared" si="346"/>
@@ -4083,11 +4057,11 @@
       </c>
       <c r="K121">
         <f t="shared" si="346"/>
-        <v>21324.142857142859</v>
+        <v>0</v>
       </c>
       <c r="L121">
         <f t="shared" si="346"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M121">
         <f t="shared" si="346"/>
@@ -4103,30 +4077,36 @@
       </c>
       <c r="C122">
         <f t="shared" si="211"/>
-        <v>55511.428571428572</v>
+        <v>60551.428571428565</v>
+      </c>
+      <c r="D122">
+        <v>208260</v>
+      </c>
+      <c r="G122">
+        <v>105600</v>
       </c>
       <c r="H122">
-        <v>388580</v>
+        <v>110000</v>
       </c>
       <c r="I122">
-        <f t="shared" ref="I122:I153" si="347">D122/7</f>
-        <v>0</v>
+        <f t="shared" ref="I122" si="347">D122/7</f>
+        <v>29751.428571428572</v>
       </c>
       <c r="J122">
-        <f t="shared" ref="J122:J153" si="348">E122/7</f>
+        <f t="shared" ref="J122" si="348">E122/7</f>
         <v>0</v>
       </c>
       <c r="K122">
-        <f t="shared" ref="K122:K153" si="349">F122/7</f>
+        <f t="shared" ref="K122" si="349">F122/7</f>
         <v>0</v>
       </c>
       <c r="L122">
-        <f t="shared" ref="L122:L153" si="350">G122/7</f>
-        <v>0</v>
+        <f t="shared" ref="L122" si="350">G122/7</f>
+        <v>15085.714285714286</v>
       </c>
       <c r="M122">
-        <f t="shared" ref="M122:M153" si="351">H122/7</f>
-        <v>55511.428571428572</v>
+        <f t="shared" ref="M122" si="351">H122/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
@@ -4135,27 +4115,27 @@
       </c>
       <c r="C123">
         <f t="shared" si="211"/>
-        <v>55511.428571428572</v>
+        <v>60551.428571428565</v>
       </c>
       <c r="I123">
-        <f t="shared" ref="I123:I154" si="352">D122/7</f>
-        <v>0</v>
+        <f t="shared" ref="I123" si="352">D122/7</f>
+        <v>29751.428571428572</v>
       </c>
       <c r="J123">
-        <f t="shared" ref="J123:J154" si="353">E122/7</f>
+        <f t="shared" ref="J123" si="353">E122/7</f>
         <v>0</v>
       </c>
       <c r="K123">
-        <f t="shared" ref="K123:K154" si="354">F122/7</f>
+        <f t="shared" ref="K123" si="354">F122/7</f>
         <v>0</v>
       </c>
       <c r="L123">
-        <f t="shared" ref="L123:L154" si="355">G122/7</f>
-        <v>0</v>
+        <f t="shared" ref="L123" si="355">G122/7</f>
+        <v>15085.714285714286</v>
       </c>
       <c r="M123">
-        <f t="shared" ref="M123:M154" si="356">H122/7</f>
-        <v>55511.428571428572</v>
+        <f t="shared" ref="M123" si="356">H122/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.3">
@@ -4164,11 +4144,11 @@
       </c>
       <c r="C124">
         <f t="shared" si="211"/>
-        <v>55511.428571428572</v>
+        <v>60551.428571428565</v>
       </c>
       <c r="I124">
         <f t="shared" ref="I124:M124" si="357">D122/7</f>
-        <v>0</v>
+        <v>29751.428571428572</v>
       </c>
       <c r="J124">
         <f t="shared" si="357"/>
@@ -4180,11 +4160,11 @@
       </c>
       <c r="L124">
         <f t="shared" si="357"/>
-        <v>0</v>
+        <v>15085.714285714286</v>
       </c>
       <c r="M124">
         <f t="shared" si="357"/>
-        <v>55511.428571428572</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">
@@ -4193,11 +4173,11 @@
       </c>
       <c r="C125">
         <f t="shared" si="211"/>
-        <v>55511.428571428572</v>
+        <v>60551.428571428565</v>
       </c>
       <c r="I125">
         <f t="shared" ref="I125:M125" si="358">D122/7</f>
-        <v>0</v>
+        <v>29751.428571428572</v>
       </c>
       <c r="J125">
         <f t="shared" si="358"/>
@@ -4209,11 +4189,11 @@
       </c>
       <c r="L125">
         <f t="shared" si="358"/>
-        <v>0</v>
+        <v>15085.714285714286</v>
       </c>
       <c r="M125">
         <f t="shared" si="358"/>
-        <v>55511.428571428572</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.3">
@@ -4222,11 +4202,11 @@
       </c>
       <c r="C126">
         <f t="shared" si="211"/>
-        <v>55511.428571428572</v>
+        <v>60551.428571428565</v>
       </c>
       <c r="I126">
         <f t="shared" ref="I126:M126" si="359">D122/7</f>
-        <v>0</v>
+        <v>29751.428571428572</v>
       </c>
       <c r="J126">
         <f t="shared" si="359"/>
@@ -4238,11 +4218,11 @@
       </c>
       <c r="L126">
         <f t="shared" si="359"/>
-        <v>0</v>
+        <v>15085.714285714286</v>
       </c>
       <c r="M126">
         <f t="shared" si="359"/>
-        <v>55511.428571428572</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.3">
@@ -4251,11 +4231,11 @@
       </c>
       <c r="C127">
         <f t="shared" si="211"/>
-        <v>55511.428571428572</v>
+        <v>60551.428571428565</v>
       </c>
       <c r="I127">
         <f t="shared" ref="I127:M127" si="360">D122/7</f>
-        <v>0</v>
+        <v>29751.428571428572</v>
       </c>
       <c r="J127">
         <f t="shared" si="360"/>
@@ -4267,11 +4247,11 @@
       </c>
       <c r="L127">
         <f t="shared" si="360"/>
-        <v>0</v>
+        <v>15085.714285714286</v>
       </c>
       <c r="M127">
         <f t="shared" si="360"/>
-        <v>55511.428571428572</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
@@ -4280,11 +4260,11 @@
       </c>
       <c r="C128">
         <f t="shared" si="211"/>
-        <v>55511.428571428572</v>
+        <v>60551.428571428565</v>
       </c>
       <c r="I128">
         <f t="shared" ref="I128:M128" si="361">D122/7</f>
-        <v>0</v>
+        <v>29751.428571428572</v>
       </c>
       <c r="J128">
         <f t="shared" si="361"/>
@@ -4296,11 +4276,11 @@
       </c>
       <c r="L128">
         <f t="shared" si="361"/>
-        <v>0</v>
+        <v>15085.714285714286</v>
       </c>
       <c r="M128">
         <f t="shared" si="361"/>
-        <v>55511.428571428572</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.3">
@@ -4312,30 +4292,33 @@
       </c>
       <c r="C129">
         <f t="shared" si="211"/>
-        <v>55511.571428571428</v>
+        <v>46301.428571428572</v>
+      </c>
+      <c r="D129">
+        <v>214110</v>
       </c>
       <c r="H129">
-        <v>388581</v>
+        <v>110000</v>
       </c>
       <c r="I129">
-        <f t="shared" ref="I129:I160" si="362">D129/7</f>
-        <v>0</v>
+        <f t="shared" ref="I129" si="362">D129/7</f>
+        <v>30587.142857142859</v>
       </c>
       <c r="J129">
-        <f t="shared" ref="J129:J160" si="363">E129/7</f>
+        <f t="shared" ref="J129" si="363">E129/7</f>
         <v>0</v>
       </c>
       <c r="K129">
-        <f t="shared" ref="K129:K160" si="364">F129/7</f>
+        <f t="shared" ref="K129" si="364">F129/7</f>
         <v>0</v>
       </c>
       <c r="L129">
-        <f t="shared" ref="L129:L160" si="365">G129/7</f>
+        <f t="shared" ref="L129" si="365">G129/7</f>
         <v>0</v>
       </c>
       <c r="M129">
-        <f t="shared" ref="M129:M160" si="366">H129/7</f>
-        <v>55511.571428571428</v>
+        <f t="shared" ref="M129" si="366">H129/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.3">
@@ -4344,27 +4327,27 @@
       </c>
       <c r="C130">
         <f t="shared" si="211"/>
-        <v>55511.571428571428</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I130">
-        <f t="shared" ref="I130:I161" si="367">D129/7</f>
-        <v>0</v>
+        <f t="shared" ref="I130" si="367">D129/7</f>
+        <v>30587.142857142859</v>
       </c>
       <c r="J130">
-        <f t="shared" ref="J130:J161" si="368">E129/7</f>
+        <f t="shared" ref="J130" si="368">E129/7</f>
         <v>0</v>
       </c>
       <c r="K130">
-        <f t="shared" ref="K130:K161" si="369">F129/7</f>
+        <f t="shared" ref="K130" si="369">F129/7</f>
         <v>0</v>
       </c>
       <c r="L130">
-        <f t="shared" ref="L130:L161" si="370">G129/7</f>
+        <f t="shared" ref="L130" si="370">G129/7</f>
         <v>0</v>
       </c>
       <c r="M130">
-        <f t="shared" ref="M130:M161" si="371">H129/7</f>
-        <v>55511.571428571428</v>
+        <f t="shared" ref="M130" si="371">H129/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
@@ -4373,11 +4356,11 @@
       </c>
       <c r="C131">
         <f t="shared" si="211"/>
-        <v>55511.571428571428</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I131">
         <f t="shared" ref="I131:M131" si="372">D129/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J131">
         <f t="shared" si="372"/>
@@ -4393,7 +4376,7 @@
       </c>
       <c r="M131">
         <f t="shared" si="372"/>
-        <v>55511.571428571428</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.3">
@@ -4402,11 +4385,11 @@
       </c>
       <c r="C132">
         <f t="shared" ref="C132:C195" si="373">SUM(I132:M132)</f>
-        <v>55511.571428571428</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I132">
         <f t="shared" ref="I132:M132" si="374">D129/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J132">
         <f t="shared" si="374"/>
@@ -4422,7 +4405,7 @@
       </c>
       <c r="M132">
         <f t="shared" si="374"/>
-        <v>55511.571428571428</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.3">
@@ -4431,11 +4414,11 @@
       </c>
       <c r="C133">
         <f t="shared" si="373"/>
-        <v>55511.571428571428</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I133">
         <f t="shared" ref="I133:M133" si="375">D129/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J133">
         <f t="shared" si="375"/>
@@ -4451,7 +4434,7 @@
       </c>
       <c r="M133">
         <f t="shared" si="375"/>
-        <v>55511.571428571428</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.3">
@@ -4460,11 +4443,11 @@
       </c>
       <c r="C134">
         <f t="shared" si="373"/>
-        <v>55511.571428571428</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I134">
         <f t="shared" ref="I134:M134" si="376">D129/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J134">
         <f t="shared" si="376"/>
@@ -4480,7 +4463,7 @@
       </c>
       <c r="M134">
         <f t="shared" si="376"/>
-        <v>55511.571428571428</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.3">
@@ -4489,11 +4472,11 @@
       </c>
       <c r="C135">
         <f t="shared" si="373"/>
-        <v>55511.571428571428</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I135">
         <f t="shared" ref="I135:M135" si="377">D129/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J135">
         <f t="shared" si="377"/>
@@ -4509,7 +4492,7 @@
       </c>
       <c r="M135">
         <f t="shared" si="377"/>
-        <v>55511.571428571428</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.3">
@@ -4521,30 +4504,33 @@
       </c>
       <c r="C136">
         <f t="shared" si="373"/>
-        <v>55511.714285714283</v>
+        <v>46301.428571428572</v>
+      </c>
+      <c r="D136">
+        <v>214110</v>
       </c>
       <c r="H136">
-        <v>388582</v>
+        <v>110000</v>
       </c>
       <c r="I136">
-        <f t="shared" ref="I136:I167" si="378">D136/7</f>
-        <v>0</v>
+        <f t="shared" ref="I136" si="378">D136/7</f>
+        <v>30587.142857142859</v>
       </c>
       <c r="J136">
-        <f t="shared" ref="J136:J167" si="379">E136/7</f>
+        <f t="shared" ref="J136" si="379">E136/7</f>
         <v>0</v>
       </c>
       <c r="K136">
-        <f t="shared" ref="K136:K167" si="380">F136/7</f>
+        <f t="shared" ref="K136" si="380">F136/7</f>
         <v>0</v>
       </c>
       <c r="L136">
-        <f t="shared" ref="L136:L167" si="381">G136/7</f>
+        <f t="shared" ref="L136" si="381">G136/7</f>
         <v>0</v>
       </c>
       <c r="M136">
-        <f t="shared" ref="M136:M167" si="382">H136/7</f>
-        <v>55511.714285714283</v>
+        <f t="shared" ref="M136" si="382">H136/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.3">
@@ -4553,27 +4539,27 @@
       </c>
       <c r="C137">
         <f t="shared" si="373"/>
-        <v>55511.714285714283</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I137">
-        <f t="shared" ref="I137:I168" si="383">D136/7</f>
-        <v>0</v>
+        <f t="shared" ref="I137" si="383">D136/7</f>
+        <v>30587.142857142859</v>
       </c>
       <c r="J137">
-        <f t="shared" ref="J137:J168" si="384">E136/7</f>
+        <f t="shared" ref="J137" si="384">E136/7</f>
         <v>0</v>
       </c>
       <c r="K137">
-        <f t="shared" ref="K137:K168" si="385">F136/7</f>
+        <f t="shared" ref="K137" si="385">F136/7</f>
         <v>0</v>
       </c>
       <c r="L137">
-        <f t="shared" ref="L137:L168" si="386">G136/7</f>
+        <f t="shared" ref="L137" si="386">G136/7</f>
         <v>0</v>
       </c>
       <c r="M137">
-        <f t="shared" ref="M137:M168" si="387">H136/7</f>
-        <v>55511.714285714283</v>
+        <f t="shared" ref="M137" si="387">H136/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.3">
@@ -4582,11 +4568,11 @@
       </c>
       <c r="C138">
         <f t="shared" si="373"/>
-        <v>55511.714285714283</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I138">
         <f t="shared" ref="I138:M138" si="388">D136/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J138">
         <f t="shared" si="388"/>
@@ -4602,7 +4588,7 @@
       </c>
       <c r="M138">
         <f t="shared" si="388"/>
-        <v>55511.714285714283</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.3">
@@ -4611,11 +4597,11 @@
       </c>
       <c r="C139">
         <f t="shared" si="373"/>
-        <v>55511.714285714283</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I139">
         <f t="shared" ref="I139:M139" si="389">D136/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J139">
         <f t="shared" si="389"/>
@@ -4631,7 +4617,7 @@
       </c>
       <c r="M139">
         <f t="shared" si="389"/>
-        <v>55511.714285714283</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.3">
@@ -4640,11 +4626,11 @@
       </c>
       <c r="C140">
         <f t="shared" si="373"/>
-        <v>55511.714285714283</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I140">
         <f t="shared" ref="I140:M140" si="390">D136/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J140">
         <f t="shared" si="390"/>
@@ -4660,7 +4646,7 @@
       </c>
       <c r="M140">
         <f t="shared" si="390"/>
-        <v>55511.714285714283</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.3">
@@ -4669,11 +4655,11 @@
       </c>
       <c r="C141">
         <f t="shared" si="373"/>
-        <v>55511.714285714283</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I141">
         <f t="shared" ref="I141:M141" si="391">D136/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J141">
         <f t="shared" si="391"/>
@@ -4689,7 +4675,7 @@
       </c>
       <c r="M141">
         <f t="shared" si="391"/>
-        <v>55511.714285714283</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.3">
@@ -4698,11 +4684,11 @@
       </c>
       <c r="C142">
         <f t="shared" si="373"/>
-        <v>55511.714285714283</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I142">
         <f t="shared" ref="I142:M142" si="392">D136/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J142">
         <f t="shared" si="392"/>
@@ -4718,7 +4704,7 @@
       </c>
       <c r="M142">
         <f t="shared" si="392"/>
-        <v>55511.714285714283</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.3">
@@ -4730,30 +4716,33 @@
       </c>
       <c r="C143">
         <f t="shared" si="373"/>
-        <v>55511.857142857145</v>
+        <v>46301.428571428572</v>
+      </c>
+      <c r="D143">
+        <v>214110</v>
       </c>
       <c r="H143">
-        <v>388583</v>
+        <v>110000</v>
       </c>
       <c r="I143">
-        <f t="shared" ref="I143:I174" si="393">D143/7</f>
-        <v>0</v>
+        <f t="shared" ref="I143" si="393">D143/7</f>
+        <v>30587.142857142859</v>
       </c>
       <c r="J143">
-        <f t="shared" ref="J143:J174" si="394">E143/7</f>
+        <f t="shared" ref="J143" si="394">E143/7</f>
         <v>0</v>
       </c>
       <c r="K143">
-        <f t="shared" ref="K143:K174" si="395">F143/7</f>
+        <f t="shared" ref="K143" si="395">F143/7</f>
         <v>0</v>
       </c>
       <c r="L143">
-        <f t="shared" ref="L143:L174" si="396">G143/7</f>
+        <f t="shared" ref="L143" si="396">G143/7</f>
         <v>0</v>
       </c>
       <c r="M143">
-        <f t="shared" ref="M143:M174" si="397">H143/7</f>
-        <v>55511.857142857145</v>
+        <f t="shared" ref="M143" si="397">H143/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.3">
@@ -4762,27 +4751,27 @@
       </c>
       <c r="C144">
         <f t="shared" si="373"/>
-        <v>55511.857142857145</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I144">
-        <f t="shared" ref="I144:I175" si="398">D143/7</f>
-        <v>0</v>
+        <f t="shared" ref="I144" si="398">D143/7</f>
+        <v>30587.142857142859</v>
       </c>
       <c r="J144">
-        <f t="shared" ref="J144:J175" si="399">E143/7</f>
+        <f t="shared" ref="J144" si="399">E143/7</f>
         <v>0</v>
       </c>
       <c r="K144">
-        <f t="shared" ref="K144:K175" si="400">F143/7</f>
+        <f t="shared" ref="K144" si="400">F143/7</f>
         <v>0</v>
       </c>
       <c r="L144">
-        <f t="shared" ref="L144:L175" si="401">G143/7</f>
+        <f t="shared" ref="L144" si="401">G143/7</f>
         <v>0</v>
       </c>
       <c r="M144">
-        <f t="shared" ref="M144:M175" si="402">H143/7</f>
-        <v>55511.857142857145</v>
+        <f t="shared" ref="M144" si="402">H143/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.3">
@@ -4791,11 +4780,11 @@
       </c>
       <c r="C145">
         <f t="shared" si="373"/>
-        <v>55511.857142857145</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I145">
         <f t="shared" ref="I145:M145" si="403">D143/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J145">
         <f t="shared" si="403"/>
@@ -4811,7 +4800,7 @@
       </c>
       <c r="M145">
         <f t="shared" si="403"/>
-        <v>55511.857142857145</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.3">
@@ -4820,11 +4809,11 @@
       </c>
       <c r="C146">
         <f t="shared" si="373"/>
-        <v>55511.857142857145</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I146">
         <f t="shared" ref="I146:M146" si="404">D143/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J146">
         <f t="shared" si="404"/>
@@ -4840,7 +4829,7 @@
       </c>
       <c r="M146">
         <f t="shared" si="404"/>
-        <v>55511.857142857145</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.3">
@@ -4849,11 +4838,11 @@
       </c>
       <c r="C147">
         <f t="shared" si="373"/>
-        <v>55511.857142857145</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I147">
         <f t="shared" ref="I147:M147" si="405">D143/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J147">
         <f t="shared" si="405"/>
@@ -4869,7 +4858,7 @@
       </c>
       <c r="M147">
         <f t="shared" si="405"/>
-        <v>55511.857142857145</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.3">
@@ -4878,11 +4867,11 @@
       </c>
       <c r="C148">
         <f t="shared" si="373"/>
-        <v>55511.857142857145</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I148">
         <f t="shared" ref="I148:M148" si="406">D143/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J148">
         <f t="shared" si="406"/>
@@ -4898,7 +4887,7 @@
       </c>
       <c r="M148">
         <f t="shared" si="406"/>
-        <v>55511.857142857145</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.3">
@@ -4907,11 +4896,11 @@
       </c>
       <c r="C149">
         <f t="shared" si="373"/>
-        <v>55511.857142857145</v>
+        <v>46301.428571428572</v>
       </c>
       <c r="I149">
         <f t="shared" ref="I149:M149" si="407">D143/7</f>
-        <v>0</v>
+        <v>30587.142857142859</v>
       </c>
       <c r="J149">
         <f t="shared" si="407"/>
@@ -4927,7 +4916,7 @@
       </c>
       <c r="M149">
         <f t="shared" si="407"/>
-        <v>55511.857142857145</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.3">
@@ -4939,30 +4928,33 @@
       </c>
       <c r="C150">
         <f t="shared" si="373"/>
-        <v>55512</v>
+        <v>58837.142857142855</v>
+      </c>
+      <c r="D150">
+        <v>301860</v>
       </c>
       <c r="H150">
-        <v>388584</v>
+        <v>110000</v>
       </c>
       <c r="I150">
-        <f t="shared" ref="I150:I181" si="408">D150/7</f>
-        <v>0</v>
+        <f t="shared" ref="I150" si="408">D150/7</f>
+        <v>43122.857142857145</v>
       </c>
       <c r="J150">
-        <f t="shared" ref="J150:J181" si="409">E150/7</f>
+        <f t="shared" ref="J150" si="409">E150/7</f>
         <v>0</v>
       </c>
       <c r="K150">
-        <f t="shared" ref="K150:K181" si="410">F150/7</f>
+        <f t="shared" ref="K150" si="410">F150/7</f>
         <v>0</v>
       </c>
       <c r="L150">
-        <f t="shared" ref="L150:L181" si="411">G150/7</f>
+        <f t="shared" ref="L150" si="411">G150/7</f>
         <v>0</v>
       </c>
       <c r="M150">
-        <f t="shared" ref="M150:M181" si="412">H150/7</f>
-        <v>55512</v>
+        <f t="shared" ref="M150" si="412">H150/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.3">
@@ -4971,27 +4963,27 @@
       </c>
       <c r="C151">
         <f t="shared" si="373"/>
-        <v>55512</v>
+        <v>58837.142857142855</v>
       </c>
       <c r="I151">
-        <f t="shared" ref="I151:I182" si="413">D150/7</f>
-        <v>0</v>
+        <f t="shared" ref="I151" si="413">D150/7</f>
+        <v>43122.857142857145</v>
       </c>
       <c r="J151">
-        <f t="shared" ref="J151:J182" si="414">E150/7</f>
+        <f t="shared" ref="J151" si="414">E150/7</f>
         <v>0</v>
       </c>
       <c r="K151">
-        <f t="shared" ref="K151:K182" si="415">F150/7</f>
+        <f t="shared" ref="K151" si="415">F150/7</f>
         <v>0</v>
       </c>
       <c r="L151">
-        <f t="shared" ref="L151:L182" si="416">G150/7</f>
+        <f t="shared" ref="L151" si="416">G150/7</f>
         <v>0</v>
       </c>
       <c r="M151">
-        <f t="shared" ref="M151:M182" si="417">H150/7</f>
-        <v>55512</v>
+        <f t="shared" ref="M151" si="417">H150/7</f>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.3">
@@ -5000,11 +4992,11 @@
       </c>
       <c r="C152">
         <f t="shared" si="373"/>
-        <v>55512</v>
+        <v>58837.142857142855</v>
       </c>
       <c r="I152">
         <f t="shared" ref="I152:M152" si="418">D150/7</f>
-        <v>0</v>
+        <v>43122.857142857145</v>
       </c>
       <c r="J152">
         <f t="shared" si="418"/>
@@ -5020,7 +5012,7 @@
       </c>
       <c r="M152">
         <f t="shared" si="418"/>
-        <v>55512</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.3">
@@ -5029,11 +5021,11 @@
       </c>
       <c r="C153">
         <f t="shared" si="373"/>
-        <v>55512</v>
+        <v>58837.142857142855</v>
       </c>
       <c r="I153">
         <f t="shared" ref="I153:M153" si="419">D150/7</f>
-        <v>0</v>
+        <v>43122.857142857145</v>
       </c>
       <c r="J153">
         <f t="shared" si="419"/>
@@ -5049,7 +5041,7 @@
       </c>
       <c r="M153">
         <f t="shared" si="419"/>
-        <v>55512</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.3">
@@ -5058,11 +5050,11 @@
       </c>
       <c r="C154">
         <f t="shared" si="373"/>
-        <v>55512</v>
+        <v>58837.142857142855</v>
       </c>
       <c r="I154">
         <f t="shared" ref="I154:M154" si="420">D150/7</f>
-        <v>0</v>
+        <v>43122.857142857145</v>
       </c>
       <c r="J154">
         <f t="shared" si="420"/>
@@ -5078,7 +5070,7 @@
       </c>
       <c r="M154">
         <f t="shared" si="420"/>
-        <v>55512</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.3">
@@ -5087,11 +5079,11 @@
       </c>
       <c r="C155">
         <f t="shared" si="373"/>
-        <v>55512</v>
+        <v>58837.142857142855</v>
       </c>
       <c r="I155">
         <f t="shared" ref="I155:M155" si="421">D150/7</f>
-        <v>0</v>
+        <v>43122.857142857145</v>
       </c>
       <c r="J155">
         <f t="shared" si="421"/>
@@ -5107,7 +5099,7 @@
       </c>
       <c r="M155">
         <f t="shared" si="421"/>
-        <v>55512</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.3">
@@ -5116,11 +5108,11 @@
       </c>
       <c r="C156">
         <f t="shared" si="373"/>
-        <v>55512</v>
+        <v>58837.142857142855</v>
       </c>
       <c r="I156">
         <f t="shared" ref="I156:M156" si="422">D150/7</f>
-        <v>0</v>
+        <v>43122.857142857145</v>
       </c>
       <c r="J156">
         <f t="shared" si="422"/>
@@ -5136,7 +5128,7 @@
       </c>
       <c r="M156">
         <f t="shared" si="422"/>
-        <v>55512</v>
+        <v>15714.285714285714</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.3">
@@ -5148,30 +5140,30 @@
       </c>
       <c r="C157">
         <f t="shared" si="373"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="H157">
-        <v>833925</v>
+        <v>787560</v>
       </c>
       <c r="I157">
-        <f t="shared" ref="I157:I188" si="423">D157/7</f>
+        <f t="shared" ref="I157" si="423">D157/7</f>
         <v>0</v>
       </c>
       <c r="J157">
-        <f t="shared" ref="J157:J188" si="424">E157/7</f>
+        <f t="shared" ref="J157" si="424">E157/7</f>
         <v>0</v>
       </c>
       <c r="K157">
-        <f t="shared" ref="K157:K188" si="425">F157/7</f>
+        <f t="shared" ref="K157" si="425">F157/7</f>
         <v>0</v>
       </c>
       <c r="L157">
-        <f t="shared" ref="L157:L188" si="426">G157/7</f>
+        <f t="shared" ref="L157" si="426">G157/7</f>
         <v>0</v>
       </c>
       <c r="M157">
-        <f t="shared" ref="M157:M188" si="427">H157/7</f>
-        <v>119132.14285714286</v>
+        <f t="shared" ref="M157" si="427">H157/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.3">
@@ -5180,27 +5172,27 @@
       </c>
       <c r="C158">
         <f t="shared" si="373"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I158">
-        <f t="shared" ref="I158:I189" si="428">D157/7</f>
+        <f t="shared" ref="I158" si="428">D157/7</f>
         <v>0</v>
       </c>
       <c r="J158">
-        <f t="shared" ref="J158:J189" si="429">E157/7</f>
+        <f t="shared" ref="J158" si="429">E157/7</f>
         <v>0</v>
       </c>
       <c r="K158">
-        <f t="shared" ref="K158:K189" si="430">F157/7</f>
+        <f t="shared" ref="K158" si="430">F157/7</f>
         <v>0</v>
       </c>
       <c r="L158">
-        <f t="shared" ref="L158:L189" si="431">G157/7</f>
+        <f t="shared" ref="L158" si="431">G157/7</f>
         <v>0</v>
       </c>
       <c r="M158">
-        <f t="shared" ref="M158:M189" si="432">H157/7</f>
-        <v>119132.14285714286</v>
+        <f t="shared" ref="M158" si="432">H157/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.3">
@@ -5209,7 +5201,7 @@
       </c>
       <c r="C159">
         <f t="shared" si="373"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I159">
         <f t="shared" ref="I159:M159" si="433">D157/7</f>
@@ -5229,7 +5221,7 @@
       </c>
       <c r="M159">
         <f t="shared" si="433"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.3">
@@ -5238,7 +5230,7 @@
       </c>
       <c r="C160">
         <f t="shared" si="373"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I160">
         <f t="shared" ref="I160:M160" si="434">D157/7</f>
@@ -5258,7 +5250,7 @@
       </c>
       <c r="M160">
         <f t="shared" si="434"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.3">
@@ -5267,7 +5259,7 @@
       </c>
       <c r="C161">
         <f t="shared" si="373"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I161">
         <f t="shared" ref="I161:M161" si="435">D157/7</f>
@@ -5287,7 +5279,7 @@
       </c>
       <c r="M161">
         <f t="shared" si="435"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.3">
@@ -5296,7 +5288,7 @@
       </c>
       <c r="C162">
         <f t="shared" si="373"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I162">
         <f t="shared" ref="I162:M162" si="436">D157/7</f>
@@ -5316,7 +5308,7 @@
       </c>
       <c r="M162">
         <f t="shared" si="436"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.3">
@@ -5325,7 +5317,7 @@
       </c>
       <c r="C163">
         <f t="shared" si="373"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I163">
         <f t="shared" ref="I163:M163" si="437">D157/7</f>
@@ -5345,7 +5337,7 @@
       </c>
       <c r="M163">
         <f t="shared" si="437"/>
-        <v>119132.14285714286</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.3">
@@ -5357,30 +5349,30 @@
       </c>
       <c r="C164">
         <f t="shared" si="373"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="H164">
-        <v>833926</v>
+        <v>787560</v>
       </c>
       <c r="I164">
-        <f t="shared" ref="I164:I195" si="438">D164/7</f>
+        <f t="shared" ref="I164" si="438">D164/7</f>
         <v>0</v>
       </c>
       <c r="J164">
-        <f t="shared" ref="J164:J195" si="439">E164/7</f>
+        <f t="shared" ref="J164" si="439">E164/7</f>
         <v>0</v>
       </c>
       <c r="K164">
-        <f t="shared" ref="K164:K195" si="440">F164/7</f>
+        <f t="shared" ref="K164" si="440">F164/7</f>
         <v>0</v>
       </c>
       <c r="L164">
-        <f t="shared" ref="L164:L195" si="441">G164/7</f>
+        <f t="shared" ref="L164" si="441">G164/7</f>
         <v>0</v>
       </c>
       <c r="M164">
-        <f t="shared" ref="M164:M195" si="442">H164/7</f>
-        <v>119132.28571428571</v>
+        <f t="shared" ref="M164" si="442">H164/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.3">
@@ -5389,27 +5381,27 @@
       </c>
       <c r="C165">
         <f t="shared" si="373"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I165">
-        <f t="shared" ref="I165:I212" si="443">D164/7</f>
+        <f t="shared" ref="I165" si="443">D164/7</f>
         <v>0</v>
       </c>
       <c r="J165">
-        <f t="shared" ref="J165:J212" si="444">E164/7</f>
+        <f t="shared" ref="J165" si="444">E164/7</f>
         <v>0</v>
       </c>
       <c r="K165">
-        <f t="shared" ref="K165:K212" si="445">F164/7</f>
+        <f t="shared" ref="K165" si="445">F164/7</f>
         <v>0</v>
       </c>
       <c r="L165">
-        <f t="shared" ref="L165:L212" si="446">G164/7</f>
+        <f t="shared" ref="L165" si="446">G164/7</f>
         <v>0</v>
       </c>
       <c r="M165">
-        <f t="shared" ref="M165:M212" si="447">H164/7</f>
-        <v>119132.28571428571</v>
+        <f t="shared" ref="M165" si="447">H164/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.3">
@@ -5418,7 +5410,7 @@
       </c>
       <c r="C166">
         <f t="shared" si="373"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I166">
         <f t="shared" ref="I166:M166" si="448">D164/7</f>
@@ -5438,7 +5430,7 @@
       </c>
       <c r="M166">
         <f t="shared" si="448"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.3">
@@ -5447,7 +5439,7 @@
       </c>
       <c r="C167">
         <f t="shared" si="373"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I167">
         <f t="shared" ref="I167:M167" si="449">D164/7</f>
@@ -5467,7 +5459,7 @@
       </c>
       <c r="M167">
         <f t="shared" si="449"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.3">
@@ -5476,7 +5468,7 @@
       </c>
       <c r="C168">
         <f t="shared" si="373"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I168">
         <f t="shared" ref="I168:M168" si="450">D164/7</f>
@@ -5496,7 +5488,7 @@
       </c>
       <c r="M168">
         <f t="shared" si="450"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.3">
@@ -5505,7 +5497,7 @@
       </c>
       <c r="C169">
         <f t="shared" si="373"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I169">
         <f t="shared" ref="I169:M169" si="451">D164/7</f>
@@ -5525,7 +5517,7 @@
       </c>
       <c r="M169">
         <f t="shared" si="451"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.3">
@@ -5534,7 +5526,7 @@
       </c>
       <c r="C170">
         <f t="shared" si="373"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I170">
         <f t="shared" ref="I170:M170" si="452">D164/7</f>
@@ -5554,7 +5546,7 @@
       </c>
       <c r="M170">
         <f t="shared" si="452"/>
-        <v>119132.28571428571</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.3">
@@ -5566,30 +5558,30 @@
       </c>
       <c r="C171">
         <f t="shared" si="373"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="H171">
-        <v>833927</v>
+        <v>787560</v>
       </c>
       <c r="I171">
-        <f t="shared" ref="I171:I212" si="453">D171/7</f>
+        <f t="shared" ref="I171" si="453">D171/7</f>
         <v>0</v>
       </c>
       <c r="J171">
-        <f t="shared" ref="J171:J212" si="454">E171/7</f>
+        <f t="shared" ref="J171" si="454">E171/7</f>
         <v>0</v>
       </c>
       <c r="K171">
-        <f t="shared" ref="K171:K212" si="455">F171/7</f>
+        <f t="shared" ref="K171" si="455">F171/7</f>
         <v>0</v>
       </c>
       <c r="L171">
-        <f t="shared" ref="L171:L212" si="456">G171/7</f>
+        <f t="shared" ref="L171" si="456">G171/7</f>
         <v>0</v>
       </c>
       <c r="M171">
-        <f t="shared" ref="M171:M212" si="457">H171/7</f>
-        <v>119132.42857142857</v>
+        <f t="shared" ref="M171" si="457">H171/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.3">
@@ -5598,27 +5590,27 @@
       </c>
       <c r="C172">
         <f t="shared" si="373"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I172">
-        <f t="shared" ref="I172:I212" si="458">D171/7</f>
+        <f t="shared" ref="I172" si="458">D171/7</f>
         <v>0</v>
       </c>
       <c r="J172">
-        <f t="shared" ref="J172:J212" si="459">E171/7</f>
+        <f t="shared" ref="J172" si="459">E171/7</f>
         <v>0</v>
       </c>
       <c r="K172">
-        <f t="shared" ref="K172:K212" si="460">F171/7</f>
+        <f t="shared" ref="K172" si="460">F171/7</f>
         <v>0</v>
       </c>
       <c r="L172">
-        <f t="shared" ref="L172:L212" si="461">G171/7</f>
+        <f t="shared" ref="L172" si="461">G171/7</f>
         <v>0</v>
       </c>
       <c r="M172">
-        <f t="shared" ref="M172:M212" si="462">H171/7</f>
-        <v>119132.42857142857</v>
+        <f t="shared" ref="M172" si="462">H171/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.3">
@@ -5627,7 +5619,7 @@
       </c>
       <c r="C173">
         <f t="shared" si="373"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I173">
         <f t="shared" ref="I173:M173" si="463">D171/7</f>
@@ -5647,7 +5639,7 @@
       </c>
       <c r="M173">
         <f t="shared" si="463"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.3">
@@ -5656,7 +5648,7 @@
       </c>
       <c r="C174">
         <f t="shared" si="373"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I174">
         <f t="shared" ref="I174:M174" si="464">D171/7</f>
@@ -5676,7 +5668,7 @@
       </c>
       <c r="M174">
         <f t="shared" si="464"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.3">
@@ -5685,7 +5677,7 @@
       </c>
       <c r="C175">
         <f t="shared" si="373"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I175">
         <f t="shared" ref="I175:M175" si="465">D171/7</f>
@@ -5705,7 +5697,7 @@
       </c>
       <c r="M175">
         <f t="shared" si="465"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.3">
@@ -5714,7 +5706,7 @@
       </c>
       <c r="C176">
         <f t="shared" si="373"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I176">
         <f t="shared" ref="I176:M176" si="466">D171/7</f>
@@ -5734,7 +5726,7 @@
       </c>
       <c r="M176">
         <f t="shared" si="466"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.3">
@@ -5743,7 +5735,7 @@
       </c>
       <c r="C177">
         <f t="shared" si="373"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I177">
         <f t="shared" ref="I177:M177" si="467">D171/7</f>
@@ -5763,7 +5755,7 @@
       </c>
       <c r="M177">
         <f t="shared" si="467"/>
-        <v>119132.42857142857</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.3">
@@ -5775,30 +5767,30 @@
       </c>
       <c r="C178">
         <f t="shared" si="373"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="H178">
-        <v>833928</v>
+        <v>787560</v>
       </c>
       <c r="I178">
-        <f t="shared" ref="I178:I212" si="468">D178/7</f>
+        <f t="shared" ref="I178" si="468">D178/7</f>
         <v>0</v>
       </c>
       <c r="J178">
-        <f t="shared" ref="J178:J212" si="469">E178/7</f>
+        <f t="shared" ref="J178" si="469">E178/7</f>
         <v>0</v>
       </c>
       <c r="K178">
-        <f t="shared" ref="K178:K212" si="470">F178/7</f>
+        <f t="shared" ref="K178" si="470">F178/7</f>
         <v>0</v>
       </c>
       <c r="L178">
-        <f t="shared" ref="L178:L212" si="471">G178/7</f>
+        <f t="shared" ref="L178" si="471">G178/7</f>
         <v>0</v>
       </c>
       <c r="M178">
-        <f t="shared" ref="M178:M212" si="472">H178/7</f>
-        <v>119132.57142857143</v>
+        <f t="shared" ref="M178" si="472">H178/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.3">
@@ -5807,27 +5799,27 @@
       </c>
       <c r="C179">
         <f t="shared" si="373"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I179">
-        <f t="shared" ref="I179:I212" si="473">D178/7</f>
+        <f t="shared" ref="I179" si="473">D178/7</f>
         <v>0</v>
       </c>
       <c r="J179">
-        <f t="shared" ref="J179:J212" si="474">E178/7</f>
+        <f t="shared" ref="J179" si="474">E178/7</f>
         <v>0</v>
       </c>
       <c r="K179">
-        <f t="shared" ref="K179:K212" si="475">F178/7</f>
+        <f t="shared" ref="K179" si="475">F178/7</f>
         <v>0</v>
       </c>
       <c r="L179">
-        <f t="shared" ref="L179:L212" si="476">G178/7</f>
+        <f t="shared" ref="L179" si="476">G178/7</f>
         <v>0</v>
       </c>
       <c r="M179">
-        <f t="shared" ref="M179:M212" si="477">H178/7</f>
-        <v>119132.57142857143</v>
+        <f t="shared" ref="M179" si="477">H178/7</f>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.3">
@@ -5836,7 +5828,7 @@
       </c>
       <c r="C180">
         <f t="shared" si="373"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I180">
         <f t="shared" ref="I180:M180" si="478">D178/7</f>
@@ -5856,7 +5848,7 @@
       </c>
       <c r="M180">
         <f t="shared" si="478"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.3">
@@ -5865,7 +5857,7 @@
       </c>
       <c r="C181">
         <f t="shared" si="373"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I181">
         <f t="shared" ref="I181:M181" si="479">D178/7</f>
@@ -5885,7 +5877,7 @@
       </c>
       <c r="M181">
         <f t="shared" si="479"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.3">
@@ -5894,7 +5886,7 @@
       </c>
       <c r="C182">
         <f t="shared" si="373"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I182">
         <f t="shared" ref="I182:M182" si="480">D178/7</f>
@@ -5914,7 +5906,7 @@
       </c>
       <c r="M182">
         <f t="shared" si="480"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.3">
@@ -5923,7 +5915,7 @@
       </c>
       <c r="C183">
         <f t="shared" si="373"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I183">
         <f t="shared" ref="I183:M183" si="481">D178/7</f>
@@ -5943,7 +5935,7 @@
       </c>
       <c r="M183">
         <f t="shared" si="481"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.3">
@@ -5952,7 +5944,7 @@
       </c>
       <c r="C184">
         <f t="shared" si="373"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
       <c r="I184">
         <f t="shared" ref="I184:M184" si="482">D178/7</f>
@@ -5972,7 +5964,7 @@
       </c>
       <c r="M184">
         <f t="shared" si="482"/>
-        <v>119132.57142857143</v>
+        <v>112508.57142857143</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.3">
@@ -5984,30 +5976,30 @@
       </c>
       <c r="C185">
         <f t="shared" si="373"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="H185">
-        <v>1281000</v>
+        <v>1156000</v>
       </c>
       <c r="I185">
-        <f t="shared" ref="I185:I212" si="483">D185/7</f>
+        <f t="shared" ref="I185" si="483">D185/7</f>
         <v>0</v>
       </c>
       <c r="J185">
-        <f t="shared" ref="J185:J212" si="484">E185/7</f>
+        <f t="shared" ref="J185" si="484">E185/7</f>
         <v>0</v>
       </c>
       <c r="K185">
-        <f t="shared" ref="K185:K212" si="485">F185/7</f>
+        <f t="shared" ref="K185" si="485">F185/7</f>
         <v>0</v>
       </c>
       <c r="L185">
-        <f t="shared" ref="L185:L212" si="486">G185/7</f>
+        <f t="shared" ref="L185" si="486">G185/7</f>
         <v>0</v>
       </c>
       <c r="M185">
-        <f t="shared" ref="M185:M212" si="487">H185/7</f>
-        <v>183000</v>
+        <f t="shared" ref="M185" si="487">H185/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.3">
@@ -6016,27 +6008,27 @@
       </c>
       <c r="C186">
         <f t="shared" si="373"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I186">
-        <f t="shared" ref="I186:I212" si="488">D185/7</f>
+        <f t="shared" ref="I186" si="488">D185/7</f>
         <v>0</v>
       </c>
       <c r="J186">
-        <f t="shared" ref="J186:J212" si="489">E185/7</f>
+        <f t="shared" ref="J186" si="489">E185/7</f>
         <v>0</v>
       </c>
       <c r="K186">
-        <f t="shared" ref="K186:K212" si="490">F185/7</f>
+        <f t="shared" ref="K186" si="490">F185/7</f>
         <v>0</v>
       </c>
       <c r="L186">
-        <f t="shared" ref="L186:L212" si="491">G185/7</f>
+        <f t="shared" ref="L186" si="491">G185/7</f>
         <v>0</v>
       </c>
       <c r="M186">
-        <f t="shared" ref="M186:M212" si="492">H185/7</f>
-        <v>183000</v>
+        <f t="shared" ref="M186" si="492">H185/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.3">
@@ -6045,7 +6037,7 @@
       </c>
       <c r="C187">
         <f t="shared" si="373"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I187">
         <f t="shared" ref="I187:M187" si="493">D185/7</f>
@@ -6065,7 +6057,7 @@
       </c>
       <c r="M187">
         <f t="shared" si="493"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.3">
@@ -6074,7 +6066,7 @@
       </c>
       <c r="C188">
         <f t="shared" si="373"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I188">
         <f t="shared" ref="I188:M188" si="494">D185/7</f>
@@ -6094,7 +6086,7 @@
       </c>
       <c r="M188">
         <f t="shared" si="494"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.3">
@@ -6103,7 +6095,7 @@
       </c>
       <c r="C189">
         <f t="shared" si="373"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I189">
         <f t="shared" ref="I189:M189" si="495">D185/7</f>
@@ -6123,7 +6115,7 @@
       </c>
       <c r="M189">
         <f t="shared" si="495"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.3">
@@ -6132,7 +6124,7 @@
       </c>
       <c r="C190">
         <f t="shared" si="373"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I190">
         <f t="shared" ref="I190:M190" si="496">D185/7</f>
@@ -6152,7 +6144,7 @@
       </c>
       <c r="M190">
         <f t="shared" si="496"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.3">
@@ -6161,7 +6153,7 @@
       </c>
       <c r="C191">
         <f t="shared" si="373"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I191">
         <f t="shared" ref="I191:M191" si="497">D185/7</f>
@@ -6181,7 +6173,7 @@
       </c>
       <c r="M191">
         <f t="shared" si="497"/>
-        <v>183000</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.3">
@@ -6193,30 +6185,30 @@
       </c>
       <c r="C192">
         <f t="shared" si="373"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="H192">
-        <v>1281001</v>
+        <v>1156000</v>
       </c>
       <c r="I192">
-        <f t="shared" ref="I192:I212" si="498">D192/7</f>
+        <f t="shared" ref="I192" si="498">D192/7</f>
         <v>0</v>
       </c>
       <c r="J192">
-        <f t="shared" ref="J192:J212" si="499">E192/7</f>
+        <f t="shared" ref="J192" si="499">E192/7</f>
         <v>0</v>
       </c>
       <c r="K192">
-        <f t="shared" ref="K192:K212" si="500">F192/7</f>
+        <f t="shared" ref="K192" si="500">F192/7</f>
         <v>0</v>
       </c>
       <c r="L192">
-        <f t="shared" ref="L192:L212" si="501">G192/7</f>
+        <f t="shared" ref="L192" si="501">G192/7</f>
         <v>0</v>
       </c>
       <c r="M192">
-        <f t="shared" ref="M192:M212" si="502">H192/7</f>
-        <v>183000.14285714287</v>
+        <f t="shared" ref="M192" si="502">H192/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.3">
@@ -6225,27 +6217,27 @@
       </c>
       <c r="C193">
         <f t="shared" si="373"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I193">
-        <f t="shared" ref="I193:I212" si="503">D192/7</f>
+        <f t="shared" ref="I193" si="503">D192/7</f>
         <v>0</v>
       </c>
       <c r="J193">
-        <f t="shared" ref="J193:J212" si="504">E192/7</f>
+        <f t="shared" ref="J193" si="504">E192/7</f>
         <v>0</v>
       </c>
       <c r="K193">
-        <f t="shared" ref="K193:K212" si="505">F192/7</f>
+        <f t="shared" ref="K193" si="505">F192/7</f>
         <v>0</v>
       </c>
       <c r="L193">
-        <f t="shared" ref="L193:L212" si="506">G192/7</f>
+        <f t="shared" ref="L193" si="506">G192/7</f>
         <v>0</v>
       </c>
       <c r="M193">
-        <f t="shared" ref="M193:M212" si="507">H192/7</f>
-        <v>183000.14285714287</v>
+        <f t="shared" ref="M193" si="507">H192/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.3">
@@ -6254,7 +6246,7 @@
       </c>
       <c r="C194">
         <f t="shared" si="373"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I194">
         <f t="shared" ref="I194:M194" si="508">D192/7</f>
@@ -6274,7 +6266,7 @@
       </c>
       <c r="M194">
         <f t="shared" si="508"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.3">
@@ -6283,7 +6275,7 @@
       </c>
       <c r="C195">
         <f t="shared" si="373"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I195">
         <f t="shared" ref="I195:M195" si="509">D192/7</f>
@@ -6303,7 +6295,7 @@
       </c>
       <c r="M195">
         <f t="shared" si="509"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.3">
@@ -6312,7 +6304,7 @@
       </c>
       <c r="C196">
         <f t="shared" ref="C196:C212" si="510">SUM(I196:M196)</f>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I196">
         <f t="shared" ref="I196:M196" si="511">D192/7</f>
@@ -6332,7 +6324,7 @@
       </c>
       <c r="M196">
         <f t="shared" si="511"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.3">
@@ -6341,7 +6333,7 @@
       </c>
       <c r="C197">
         <f t="shared" si="510"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I197">
         <f t="shared" ref="I197:M197" si="512">D192/7</f>
@@ -6361,7 +6353,7 @@
       </c>
       <c r="M197">
         <f t="shared" si="512"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.3">
@@ -6370,7 +6362,7 @@
       </c>
       <c r="C198">
         <f t="shared" si="510"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I198">
         <f t="shared" ref="I198:M198" si="513">D192/7</f>
@@ -6390,7 +6382,7 @@
       </c>
       <c r="M198">
         <f t="shared" si="513"/>
-        <v>183000.14285714287</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.3">
@@ -6402,30 +6394,30 @@
       </c>
       <c r="C199">
         <f t="shared" si="510"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="H199">
-        <v>1281002</v>
+        <v>1156000</v>
       </c>
       <c r="I199">
-        <f t="shared" ref="I199:I212" si="514">D199/7</f>
+        <f t="shared" ref="I199" si="514">D199/7</f>
         <v>0</v>
       </c>
       <c r="J199">
-        <f t="shared" ref="J199:J212" si="515">E199/7</f>
+        <f t="shared" ref="J199" si="515">E199/7</f>
         <v>0</v>
       </c>
       <c r="K199">
-        <f t="shared" ref="K199:K212" si="516">F199/7</f>
+        <f t="shared" ref="K199" si="516">F199/7</f>
         <v>0</v>
       </c>
       <c r="L199">
-        <f t="shared" ref="L199:L212" si="517">G199/7</f>
+        <f t="shared" ref="L199" si="517">G199/7</f>
         <v>0</v>
       </c>
       <c r="M199">
-        <f t="shared" ref="M199:M212" si="518">H199/7</f>
-        <v>183000.28571428571</v>
+        <f t="shared" ref="M199" si="518">H199/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.3">
@@ -6434,27 +6426,27 @@
       </c>
       <c r="C200">
         <f t="shared" si="510"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I200">
-        <f t="shared" ref="I200:I212" si="519">D199/7</f>
+        <f t="shared" ref="I200" si="519">D199/7</f>
         <v>0</v>
       </c>
       <c r="J200">
-        <f t="shared" ref="J200:J212" si="520">E199/7</f>
+        <f t="shared" ref="J200" si="520">E199/7</f>
         <v>0</v>
       </c>
       <c r="K200">
-        <f t="shared" ref="K200:K212" si="521">F199/7</f>
+        <f t="shared" ref="K200" si="521">F199/7</f>
         <v>0</v>
       </c>
       <c r="L200">
-        <f t="shared" ref="L200:L212" si="522">G199/7</f>
+        <f t="shared" ref="L200" si="522">G199/7</f>
         <v>0</v>
       </c>
       <c r="M200">
-        <f t="shared" ref="M200:M212" si="523">H199/7</f>
-        <v>183000.28571428571</v>
+        <f t="shared" ref="M200" si="523">H199/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.3">
@@ -6463,7 +6455,7 @@
       </c>
       <c r="C201">
         <f t="shared" si="510"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I201">
         <f t="shared" ref="I201:M201" si="524">D199/7</f>
@@ -6483,7 +6475,7 @@
       </c>
       <c r="M201">
         <f t="shared" si="524"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.3">
@@ -6492,7 +6484,7 @@
       </c>
       <c r="C202">
         <f t="shared" si="510"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I202">
         <f t="shared" ref="I202:M202" si="525">D199/7</f>
@@ -6512,7 +6504,7 @@
       </c>
       <c r="M202">
         <f t="shared" si="525"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.3">
@@ -6521,7 +6513,7 @@
       </c>
       <c r="C203">
         <f t="shared" si="510"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I203">
         <f t="shared" ref="I203:M203" si="526">D199/7</f>
@@ -6541,7 +6533,7 @@
       </c>
       <c r="M203">
         <f t="shared" si="526"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.3">
@@ -6550,7 +6542,7 @@
       </c>
       <c r="C204">
         <f t="shared" si="510"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I204">
         <f t="shared" ref="I204:M204" si="527">D199/7</f>
@@ -6570,7 +6562,7 @@
       </c>
       <c r="M204">
         <f t="shared" si="527"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.3">
@@ -6579,7 +6571,7 @@
       </c>
       <c r="C205">
         <f t="shared" si="510"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I205">
         <f t="shared" ref="I205:M205" si="528">D199/7</f>
@@ -6599,7 +6591,7 @@
       </c>
       <c r="M205">
         <f t="shared" si="528"/>
-        <v>183000.28571428571</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.3">
@@ -6611,30 +6603,30 @@
       </c>
       <c r="C206">
         <f t="shared" si="510"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="H206">
-        <v>1281003</v>
+        <v>1156000</v>
       </c>
       <c r="I206">
-        <f t="shared" ref="I206:I212" si="529">D206/7</f>
+        <f t="shared" ref="I206" si="529">D206/7</f>
         <v>0</v>
       </c>
       <c r="J206">
-        <f t="shared" ref="J206:J212" si="530">E206/7</f>
+        <f t="shared" ref="J206" si="530">E206/7</f>
         <v>0</v>
       </c>
       <c r="K206">
-        <f t="shared" ref="K206:K212" si="531">F206/7</f>
+        <f t="shared" ref="K206" si="531">F206/7</f>
         <v>0</v>
       </c>
       <c r="L206">
-        <f t="shared" ref="L206:L212" si="532">G206/7</f>
+        <f t="shared" ref="L206" si="532">G206/7</f>
         <v>0</v>
       </c>
       <c r="M206">
-        <f t="shared" ref="M206:M212" si="533">H206/7</f>
-        <v>183000.42857142858</v>
+        <f t="shared" ref="M206" si="533">H206/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.3">
@@ -6643,27 +6635,27 @@
       </c>
       <c r="C207">
         <f t="shared" si="510"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I207">
-        <f t="shared" ref="I207:I212" si="534">D206/7</f>
+        <f t="shared" ref="I207" si="534">D206/7</f>
         <v>0</v>
       </c>
       <c r="J207">
-        <f t="shared" ref="J207:J212" si="535">E206/7</f>
+        <f t="shared" ref="J207" si="535">E206/7</f>
         <v>0</v>
       </c>
       <c r="K207">
-        <f t="shared" ref="K207:K212" si="536">F206/7</f>
+        <f t="shared" ref="K207" si="536">F206/7</f>
         <v>0</v>
       </c>
       <c r="L207">
-        <f t="shared" ref="L207:L212" si="537">G206/7</f>
+        <f t="shared" ref="L207" si="537">G206/7</f>
         <v>0</v>
       </c>
       <c r="M207">
-        <f t="shared" ref="M207:M212" si="538">H206/7</f>
-        <v>183000.42857142858</v>
+        <f t="shared" ref="M207" si="538">H206/7</f>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.3">
@@ -6672,7 +6664,7 @@
       </c>
       <c r="C208">
         <f t="shared" si="510"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I208">
         <f t="shared" ref="I208:M208" si="539">D206/7</f>
@@ -6692,7 +6684,7 @@
       </c>
       <c r="M208">
         <f t="shared" si="539"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.3">
@@ -6701,7 +6693,7 @@
       </c>
       <c r="C209">
         <f t="shared" si="510"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I209">
         <f t="shared" ref="I209:M209" si="540">D206/7</f>
@@ -6721,7 +6713,7 @@
       </c>
       <c r="M209">
         <f t="shared" si="540"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.3">
@@ -6730,7 +6722,7 @@
       </c>
       <c r="C210">
         <f t="shared" si="510"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I210">
         <f t="shared" ref="I210:M210" si="541">D206/7</f>
@@ -6750,7 +6742,7 @@
       </c>
       <c r="M210">
         <f t="shared" si="541"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.3">
@@ -6759,7 +6751,7 @@
       </c>
       <c r="C211">
         <f t="shared" si="510"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I211">
         <f t="shared" ref="I211:M211" si="542">D206/7</f>
@@ -6779,7 +6771,7 @@
       </c>
       <c r="M211">
         <f t="shared" si="542"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.3">
@@ -6788,7 +6780,7 @@
       </c>
       <c r="C212">
         <f t="shared" si="510"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
       <c r="I212">
         <f t="shared" ref="I212:M212" si="543">D206/7</f>
@@ -6808,7 +6800,7 @@
       </c>
       <c r="M212">
         <f t="shared" si="543"/>
-        <v>183000.42857142858</v>
+        <v>165142.85714285713</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated vaccine calender data
</commit_message>
<xml_diff>
--- a/data/Vaccine prognoser (jan-juli).xlsx
+++ b/data/Vaccine prognoser (jan-juli).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alboa\Documents\GitHub\covid-19-modelling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8758DCFD-ACD4-4047-88E7-14852A69B746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BC0957-CF18-42FA-A6EB-76D0430CD3B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9612" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{147A47B0-1836-4FF1-9A54-614DDF6AFE19}"/>
+    <workbookView xWindow="0" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{147A47B0-1836-4FF1-9A54-614DDF6AFE19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E072CA-4E92-41AA-9440-0406EC20240D}">
   <dimension ref="A2:M226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B194" workbookViewId="0">
-      <selection activeCell="G210" sqref="G210"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="F185" sqref="F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3234,22 +3234,22 @@
       </c>
       <c r="C94">
         <f t="shared" si="211"/>
-        <v>35078.571428571428</v>
+        <v>33720</v>
       </c>
       <c r="D94">
-        <v>204750</v>
+        <v>201240</v>
       </c>
       <c r="E94">
-        <v>40800</v>
+        <v>34800</v>
       </c>
       <c r="F94" s="2"/>
       <c r="I94">
         <f t="shared" ref="I94" si="287">D94/7</f>
-        <v>29250</v>
+        <v>28748.571428571428</v>
       </c>
       <c r="J94">
         <f t="shared" ref="J94" si="288">E94/7</f>
-        <v>5828.5714285714284</v>
+        <v>4971.4285714285716</v>
       </c>
       <c r="K94">
         <f t="shared" ref="K94" si="289">F94/7</f>
@@ -3270,15 +3270,15 @@
       </c>
       <c r="C95">
         <f t="shared" si="211"/>
-        <v>35078.571428571428</v>
+        <v>33720</v>
       </c>
       <c r="I95">
         <f t="shared" ref="I95" si="292">D94/7</f>
-        <v>29250</v>
+        <v>28748.571428571428</v>
       </c>
       <c r="J95">
         <f t="shared" ref="J95" si="293">E94/7</f>
-        <v>5828.5714285714284</v>
+        <v>4971.4285714285716</v>
       </c>
       <c r="K95">
         <f t="shared" ref="K95" si="294">F94/7</f>
@@ -3299,15 +3299,15 @@
       </c>
       <c r="C96">
         <f t="shared" si="211"/>
-        <v>35078.571428571428</v>
+        <v>33720</v>
       </c>
       <c r="I96">
         <f t="shared" ref="I96:M96" si="297">D94/7</f>
-        <v>29250</v>
+        <v>28748.571428571428</v>
       </c>
       <c r="J96">
         <f t="shared" si="297"/>
-        <v>5828.5714285714284</v>
+        <v>4971.4285714285716</v>
       </c>
       <c r="K96">
         <f t="shared" si="297"/>
@@ -3328,15 +3328,15 @@
       </c>
       <c r="C97">
         <f t="shared" si="211"/>
-        <v>35078.571428571428</v>
+        <v>33720</v>
       </c>
       <c r="I97">
         <f t="shared" ref="I97:M97" si="298">D94/7</f>
-        <v>29250</v>
+        <v>28748.571428571428</v>
       </c>
       <c r="J97">
         <f t="shared" si="298"/>
-        <v>5828.5714285714284</v>
+        <v>4971.4285714285716</v>
       </c>
       <c r="K97">
         <f t="shared" si="298"/>
@@ -3357,15 +3357,15 @@
       </c>
       <c r="C98">
         <f t="shared" si="211"/>
-        <v>35078.571428571428</v>
+        <v>33720</v>
       </c>
       <c r="I98">
         <f t="shared" ref="I98:M98" si="299">D94/7</f>
-        <v>29250</v>
+        <v>28748.571428571428</v>
       </c>
       <c r="J98">
         <f t="shared" si="299"/>
-        <v>5828.5714285714284</v>
+        <v>4971.4285714285716</v>
       </c>
       <c r="K98">
         <f t="shared" si="299"/>
@@ -3386,15 +3386,15 @@
       </c>
       <c r="C99">
         <f t="shared" si="211"/>
-        <v>35078.571428571428</v>
+        <v>33720</v>
       </c>
       <c r="I99">
         <f t="shared" ref="I99:M99" si="300">D94/7</f>
-        <v>29250</v>
+        <v>28748.571428571428</v>
       </c>
       <c r="J99">
         <f t="shared" si="300"/>
-        <v>5828.5714285714284</v>
+        <v>4971.4285714285716</v>
       </c>
       <c r="K99">
         <f t="shared" si="300"/>
@@ -3415,15 +3415,15 @@
       </c>
       <c r="C100">
         <f t="shared" si="211"/>
-        <v>35078.571428571428</v>
+        <v>33720</v>
       </c>
       <c r="I100">
         <f t="shared" ref="I100:M100" si="301">D94/7</f>
-        <v>29250</v>
+        <v>28748.571428571428</v>
       </c>
       <c r="J100">
         <f t="shared" si="301"/>
-        <v>5828.5714285714284</v>
+        <v>4971.4285714285716</v>
       </c>
       <c r="K100">
         <f t="shared" si="301"/>
@@ -3656,21 +3656,21 @@
       </c>
       <c r="C108">
         <f t="shared" si="211"/>
-        <v>35760</v>
-      </c>
-      <c r="D108">
-        <v>205920</v>
+        <v>31838.571428571431</v>
+      </c>
+      <c r="D108" s="2">
+        <v>200070</v>
       </c>
       <c r="E108">
-        <v>44400</v>
+        <v>22800</v>
       </c>
       <c r="I108">
         <f t="shared" ref="I108" si="317">D108/7</f>
-        <v>29417.142857142859</v>
+        <v>28581.428571428572</v>
       </c>
       <c r="J108">
         <f t="shared" ref="J108" si="318">E108/7</f>
-        <v>6342.8571428571431</v>
+        <v>3257.1428571428573</v>
       </c>
       <c r="K108">
         <f t="shared" ref="K108" si="319">F108/7</f>
@@ -3691,15 +3691,15 @@
       </c>
       <c r="C109">
         <f t="shared" si="211"/>
-        <v>35760</v>
+        <v>31838.571428571431</v>
       </c>
       <c r="I109">
         <f t="shared" ref="I109" si="322">D108/7</f>
-        <v>29417.142857142859</v>
+        <v>28581.428571428572</v>
       </c>
       <c r="J109">
         <f t="shared" ref="J109" si="323">E108/7</f>
-        <v>6342.8571428571431</v>
+        <v>3257.1428571428573</v>
       </c>
       <c r="K109">
         <f t="shared" ref="K109" si="324">F108/7</f>
@@ -3720,15 +3720,15 @@
       </c>
       <c r="C110">
         <f t="shared" si="211"/>
-        <v>35760</v>
+        <v>31838.571428571431</v>
       </c>
       <c r="I110">
         <f t="shared" ref="I110:M110" si="327">D108/7</f>
-        <v>29417.142857142859</v>
+        <v>28581.428571428572</v>
       </c>
       <c r="J110">
         <f t="shared" si="327"/>
-        <v>6342.8571428571431</v>
+        <v>3257.1428571428573</v>
       </c>
       <c r="K110">
         <f t="shared" si="327"/>
@@ -3749,15 +3749,15 @@
       </c>
       <c r="C111">
         <f t="shared" si="211"/>
-        <v>35760</v>
+        <v>31838.571428571431</v>
       </c>
       <c r="I111">
         <f t="shared" ref="I111:M111" si="328">D108/7</f>
-        <v>29417.142857142859</v>
+        <v>28581.428571428572</v>
       </c>
       <c r="J111">
         <f t="shared" si="328"/>
-        <v>6342.8571428571431</v>
+        <v>3257.1428571428573</v>
       </c>
       <c r="K111">
         <f t="shared" si="328"/>
@@ -3778,15 +3778,15 @@
       </c>
       <c r="C112">
         <f t="shared" si="211"/>
-        <v>35760</v>
+        <v>31838.571428571431</v>
       </c>
       <c r="I112">
         <f t="shared" ref="I112:M112" si="329">D108/7</f>
-        <v>29417.142857142859</v>
+        <v>28581.428571428572</v>
       </c>
       <c r="J112">
         <f t="shared" si="329"/>
-        <v>6342.8571428571431</v>
+        <v>3257.1428571428573</v>
       </c>
       <c r="K112">
         <f t="shared" si="329"/>
@@ -3807,15 +3807,15 @@
       </c>
       <c r="C113">
         <f t="shared" si="211"/>
-        <v>35760</v>
+        <v>31838.571428571431</v>
       </c>
       <c r="I113">
         <f t="shared" ref="I113:M113" si="330">D108/7</f>
-        <v>29417.142857142859</v>
+        <v>28581.428571428572</v>
       </c>
       <c r="J113">
         <f t="shared" si="330"/>
-        <v>6342.8571428571431</v>
+        <v>3257.1428571428573</v>
       </c>
       <c r="K113">
         <f t="shared" si="330"/>
@@ -3836,15 +3836,15 @@
       </c>
       <c r="C114">
         <f t="shared" si="211"/>
-        <v>35760</v>
+        <v>31838.571428571431</v>
       </c>
       <c r="I114">
         <f t="shared" ref="I114:M114" si="331">D108/7</f>
-        <v>29417.142857142859</v>
+        <v>28581.428571428572</v>
       </c>
       <c r="J114">
         <f t="shared" si="331"/>
-        <v>6342.8571428571431</v>
+        <v>3257.1428571428573</v>
       </c>
       <c r="K114">
         <f t="shared" si="331"/>
@@ -3868,18 +3868,21 @@
       </c>
       <c r="C115">
         <f t="shared" si="211"/>
-        <v>29417.142857142859</v>
-      </c>
-      <c r="D115">
-        <v>205920</v>
+        <v>42172.857142857145</v>
+      </c>
+      <c r="D115" s="2">
+        <v>272610</v>
+      </c>
+      <c r="E115">
+        <v>22600</v>
       </c>
       <c r="I115">
         <f t="shared" ref="I115" si="332">D115/7</f>
-        <v>29417.142857142859</v>
+        <v>38944.285714285717</v>
       </c>
       <c r="J115">
         <f t="shared" ref="J115" si="333">E115/7</f>
-        <v>0</v>
+        <v>3228.5714285714284</v>
       </c>
       <c r="K115">
         <f t="shared" ref="K115" si="334">F115/7</f>
@@ -3900,15 +3903,15 @@
       </c>
       <c r="C116">
         <f t="shared" si="211"/>
-        <v>29417.142857142859</v>
+        <v>42172.857142857145</v>
       </c>
       <c r="I116">
         <f t="shared" ref="I116" si="337">D115/7</f>
-        <v>29417.142857142859</v>
+        <v>38944.285714285717</v>
       </c>
       <c r="J116">
         <f t="shared" ref="J116" si="338">E115/7</f>
-        <v>0</v>
+        <v>3228.5714285714284</v>
       </c>
       <c r="K116">
         <f t="shared" ref="K116" si="339">F115/7</f>
@@ -3929,15 +3932,15 @@
       </c>
       <c r="C117">
         <f t="shared" si="211"/>
-        <v>29417.142857142859</v>
+        <v>42172.857142857145</v>
       </c>
       <c r="I117">
         <f t="shared" ref="I117:M117" si="342">D115/7</f>
-        <v>29417.142857142859</v>
+        <v>38944.285714285717</v>
       </c>
       <c r="J117">
         <f t="shared" si="342"/>
-        <v>0</v>
+        <v>3228.5714285714284</v>
       </c>
       <c r="K117">
         <f t="shared" si="342"/>
@@ -3958,15 +3961,15 @@
       </c>
       <c r="C118">
         <f t="shared" si="211"/>
-        <v>29417.142857142859</v>
+        <v>42172.857142857145</v>
       </c>
       <c r="I118">
         <f t="shared" ref="I118:M118" si="343">D115/7</f>
-        <v>29417.142857142859</v>
+        <v>38944.285714285717</v>
       </c>
       <c r="J118">
         <f t="shared" si="343"/>
-        <v>0</v>
+        <v>3228.5714285714284</v>
       </c>
       <c r="K118">
         <f t="shared" si="343"/>
@@ -3987,15 +3990,15 @@
       </c>
       <c r="C119">
         <f t="shared" si="211"/>
-        <v>29417.142857142859</v>
+        <v>42172.857142857145</v>
       </c>
       <c r="I119">
         <f t="shared" ref="I119:M119" si="344">D115/7</f>
-        <v>29417.142857142859</v>
+        <v>38944.285714285717</v>
       </c>
       <c r="J119">
         <f t="shared" si="344"/>
-        <v>0</v>
+        <v>3228.5714285714284</v>
       </c>
       <c r="K119">
         <f t="shared" si="344"/>
@@ -4016,15 +4019,15 @@
       </c>
       <c r="C120">
         <f t="shared" si="211"/>
-        <v>29417.142857142859</v>
+        <v>42172.857142857145</v>
       </c>
       <c r="I120">
         <f t="shared" ref="I120:M120" si="345">D115/7</f>
-        <v>29417.142857142859</v>
+        <v>38944.285714285717</v>
       </c>
       <c r="J120">
         <f t="shared" si="345"/>
-        <v>0</v>
+        <v>3228.5714285714284</v>
       </c>
       <c r="K120">
         <f t="shared" si="345"/>
@@ -4045,15 +4048,15 @@
       </c>
       <c r="C121">
         <f t="shared" si="211"/>
-        <v>29417.142857142859</v>
+        <v>42172.857142857145</v>
       </c>
       <c r="I121">
         <f t="shared" ref="I121:M121" si="346">D115/7</f>
-        <v>29417.142857142859</v>
+        <v>38944.285714285717</v>
       </c>
       <c r="J121">
         <f t="shared" si="346"/>
-        <v>0</v>
+        <v>3228.5714285714284</v>
       </c>
       <c r="K121">
         <f t="shared" si="346"/>
@@ -4077,24 +4080,21 @@
       </c>
       <c r="C122">
         <f t="shared" si="211"/>
-        <v>60551.428571428565</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="D122">
-        <v>208260</v>
-      </c>
-      <c r="G122">
-        <v>105600</v>
-      </c>
-      <c r="H122">
-        <v>110000</v>
+        <v>267930</v>
+      </c>
+      <c r="E122">
+        <v>32400</v>
       </c>
       <c r="I122">
         <f t="shared" ref="I122" si="347">D122/7</f>
-        <v>29751.428571428572</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J122">
         <f t="shared" ref="J122" si="348">E122/7</f>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K122">
         <f t="shared" ref="K122" si="349">F122/7</f>
@@ -4102,11 +4102,11 @@
       </c>
       <c r="L122">
         <f t="shared" ref="L122" si="350">G122/7</f>
-        <v>15085.714285714286</v>
+        <v>0</v>
       </c>
       <c r="M122">
         <f t="shared" ref="M122" si="351">H122/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
@@ -4115,15 +4115,15 @@
       </c>
       <c r="C123">
         <f t="shared" si="211"/>
-        <v>60551.428571428565</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I123">
         <f t="shared" ref="I123" si="352">D122/7</f>
-        <v>29751.428571428572</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J123">
         <f t="shared" ref="J123" si="353">E122/7</f>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K123">
         <f t="shared" ref="K123" si="354">F122/7</f>
@@ -4131,11 +4131,11 @@
       </c>
       <c r="L123">
         <f t="shared" ref="L123" si="355">G122/7</f>
-        <v>15085.714285714286</v>
+        <v>0</v>
       </c>
       <c r="M123">
         <f t="shared" ref="M123" si="356">H122/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.3">
@@ -4144,15 +4144,15 @@
       </c>
       <c r="C124">
         <f t="shared" si="211"/>
-        <v>60551.428571428565</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I124">
         <f t="shared" ref="I124:M124" si="357">D122/7</f>
-        <v>29751.428571428572</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J124">
         <f t="shared" si="357"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K124">
         <f t="shared" si="357"/>
@@ -4160,11 +4160,11 @@
       </c>
       <c r="L124">
         <f t="shared" si="357"/>
-        <v>15085.714285714286</v>
+        <v>0</v>
       </c>
       <c r="M124">
         <f t="shared" si="357"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">
@@ -4173,15 +4173,15 @@
       </c>
       <c r="C125">
         <f t="shared" si="211"/>
-        <v>60551.428571428565</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I125">
         <f t="shared" ref="I125:M125" si="358">D122/7</f>
-        <v>29751.428571428572</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J125">
         <f t="shared" si="358"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K125">
         <f t="shared" si="358"/>
@@ -4189,11 +4189,11 @@
       </c>
       <c r="L125">
         <f t="shared" si="358"/>
-        <v>15085.714285714286</v>
+        <v>0</v>
       </c>
       <c r="M125">
         <f t="shared" si="358"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.3">
@@ -4202,15 +4202,15 @@
       </c>
       <c r="C126">
         <f t="shared" si="211"/>
-        <v>60551.428571428565</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I126">
         <f t="shared" ref="I126:M126" si="359">D122/7</f>
-        <v>29751.428571428572</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J126">
         <f t="shared" si="359"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K126">
         <f t="shared" si="359"/>
@@ -4218,11 +4218,11 @@
       </c>
       <c r="L126">
         <f t="shared" si="359"/>
-        <v>15085.714285714286</v>
+        <v>0</v>
       </c>
       <c r="M126">
         <f t="shared" si="359"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.3">
@@ -4231,15 +4231,15 @@
       </c>
       <c r="C127">
         <f t="shared" si="211"/>
-        <v>60551.428571428565</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I127">
         <f t="shared" ref="I127:M127" si="360">D122/7</f>
-        <v>29751.428571428572</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J127">
         <f t="shared" si="360"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K127">
         <f t="shared" si="360"/>
@@ -4247,11 +4247,11 @@
       </c>
       <c r="L127">
         <f t="shared" si="360"/>
-        <v>15085.714285714286</v>
+        <v>0</v>
       </c>
       <c r="M127">
         <f t="shared" si="360"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
@@ -4260,15 +4260,15 @@
       </c>
       <c r="C128">
         <f t="shared" si="211"/>
-        <v>60551.428571428565</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I128">
         <f t="shared" ref="I128:M128" si="361">D122/7</f>
-        <v>29751.428571428572</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J128">
         <f t="shared" si="361"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K128">
         <f t="shared" si="361"/>
@@ -4276,11 +4276,11 @@
       </c>
       <c r="L128">
         <f t="shared" si="361"/>
-        <v>15085.714285714286</v>
+        <v>0</v>
       </c>
       <c r="M128">
         <f t="shared" si="361"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.3">
@@ -4292,21 +4292,21 @@
       </c>
       <c r="C129">
         <f t="shared" si="211"/>
-        <v>46301.428571428572</v>
+        <v>44597.142857142855</v>
       </c>
       <c r="D129">
-        <v>214110</v>
-      </c>
-      <c r="H129">
-        <v>110000</v>
+        <v>273780</v>
+      </c>
+      <c r="E129">
+        <v>38400</v>
       </c>
       <c r="I129">
         <f t="shared" ref="I129" si="362">D129/7</f>
-        <v>30587.142857142859</v>
+        <v>39111.428571428572</v>
       </c>
       <c r="J129">
         <f t="shared" ref="J129" si="363">E129/7</f>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K129">
         <f t="shared" ref="K129" si="364">F129/7</f>
@@ -4318,7 +4318,7 @@
       </c>
       <c r="M129">
         <f t="shared" ref="M129" si="366">H129/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.3">
@@ -4327,15 +4327,15 @@
       </c>
       <c r="C130">
         <f t="shared" si="211"/>
-        <v>46301.428571428572</v>
+        <v>44597.142857142855</v>
       </c>
       <c r="I130">
         <f t="shared" ref="I130" si="367">D129/7</f>
-        <v>30587.142857142859</v>
+        <v>39111.428571428572</v>
       </c>
       <c r="J130">
         <f t="shared" ref="J130" si="368">E129/7</f>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K130">
         <f t="shared" ref="K130" si="369">F129/7</f>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="M130">
         <f t="shared" ref="M130" si="371">H129/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
@@ -4356,15 +4356,15 @@
       </c>
       <c r="C131">
         <f t="shared" si="211"/>
-        <v>46301.428571428572</v>
+        <v>44597.142857142855</v>
       </c>
       <c r="I131">
         <f t="shared" ref="I131:M131" si="372">D129/7</f>
-        <v>30587.142857142859</v>
+        <v>39111.428571428572</v>
       </c>
       <c r="J131">
         <f t="shared" si="372"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K131">
         <f t="shared" si="372"/>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="M131">
         <f t="shared" si="372"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.3">
@@ -4385,15 +4385,15 @@
       </c>
       <c r="C132">
         <f t="shared" ref="C132:C195" si="373">SUM(I132:M132)</f>
-        <v>46301.428571428572</v>
+        <v>44597.142857142855</v>
       </c>
       <c r="I132">
         <f t="shared" ref="I132:M132" si="374">D129/7</f>
-        <v>30587.142857142859</v>
+        <v>39111.428571428572</v>
       </c>
       <c r="J132">
         <f t="shared" si="374"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K132">
         <f t="shared" si="374"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="M132">
         <f t="shared" si="374"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.3">
@@ -4414,15 +4414,15 @@
       </c>
       <c r="C133">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44597.142857142855</v>
       </c>
       <c r="I133">
         <f t="shared" ref="I133:M133" si="375">D129/7</f>
-        <v>30587.142857142859</v>
+        <v>39111.428571428572</v>
       </c>
       <c r="J133">
         <f t="shared" si="375"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K133">
         <f t="shared" si="375"/>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="M133">
         <f t="shared" si="375"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.3">
@@ -4443,15 +4443,15 @@
       </c>
       <c r="C134">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44597.142857142855</v>
       </c>
       <c r="I134">
         <f t="shared" ref="I134:M134" si="376">D129/7</f>
-        <v>30587.142857142859</v>
+        <v>39111.428571428572</v>
       </c>
       <c r="J134">
         <f t="shared" si="376"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K134">
         <f t="shared" si="376"/>
@@ -4463,7 +4463,7 @@
       </c>
       <c r="M134">
         <f t="shared" si="376"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.3">
@@ -4472,15 +4472,15 @@
       </c>
       <c r="C135">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44597.142857142855</v>
       </c>
       <c r="I135">
         <f t="shared" ref="I135:M135" si="377">D129/7</f>
-        <v>30587.142857142859</v>
+        <v>39111.428571428572</v>
       </c>
       <c r="J135">
         <f t="shared" si="377"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K135">
         <f t="shared" si="377"/>
@@ -4492,7 +4492,7 @@
       </c>
       <c r="M135">
         <f t="shared" si="377"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.3">
@@ -4504,21 +4504,21 @@
       </c>
       <c r="C136">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="D136">
-        <v>214110</v>
-      </c>
-      <c r="H136">
-        <v>110000</v>
+        <v>267930</v>
+      </c>
+      <c r="E136">
+        <v>32400</v>
       </c>
       <c r="I136">
         <f t="shared" ref="I136" si="378">D136/7</f>
-        <v>30587.142857142859</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J136">
         <f t="shared" ref="J136" si="379">E136/7</f>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K136">
         <f t="shared" ref="K136" si="380">F136/7</f>
@@ -4530,7 +4530,7 @@
       </c>
       <c r="M136">
         <f t="shared" ref="M136" si="382">H136/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.3">
@@ -4539,15 +4539,15 @@
       </c>
       <c r="C137">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I137">
         <f t="shared" ref="I137" si="383">D136/7</f>
-        <v>30587.142857142859</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J137">
         <f t="shared" ref="J137" si="384">E136/7</f>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K137">
         <f t="shared" ref="K137" si="385">F136/7</f>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="M137">
         <f t="shared" ref="M137" si="387">H136/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.3">
@@ -4568,15 +4568,15 @@
       </c>
       <c r="C138">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I138">
         <f t="shared" ref="I138:M138" si="388">D136/7</f>
-        <v>30587.142857142859</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J138">
         <f t="shared" si="388"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K138">
         <f t="shared" si="388"/>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="M138">
         <f t="shared" si="388"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.3">
@@ -4597,15 +4597,15 @@
       </c>
       <c r="C139">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I139">
         <f t="shared" ref="I139:M139" si="389">D136/7</f>
-        <v>30587.142857142859</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J139">
         <f t="shared" si="389"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K139">
         <f t="shared" si="389"/>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="M139">
         <f t="shared" si="389"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.3">
@@ -4626,15 +4626,15 @@
       </c>
       <c r="C140">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I140">
         <f t="shared" ref="I140:M140" si="390">D136/7</f>
-        <v>30587.142857142859</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J140">
         <f t="shared" si="390"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K140">
         <f t="shared" si="390"/>
@@ -4646,7 +4646,7 @@
       </c>
       <c r="M140">
         <f t="shared" si="390"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.3">
@@ -4655,15 +4655,15 @@
       </c>
       <c r="C141">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I141">
         <f t="shared" ref="I141:M141" si="391">D136/7</f>
-        <v>30587.142857142859</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J141">
         <f t="shared" si="391"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K141">
         <f t="shared" si="391"/>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="M141">
         <f t="shared" si="391"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.3">
@@ -4684,15 +4684,15 @@
       </c>
       <c r="C142">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>42904.28571428571</v>
       </c>
       <c r="I142">
         <f t="shared" ref="I142:M142" si="392">D136/7</f>
-        <v>30587.142857142859</v>
+        <v>38275.714285714283</v>
       </c>
       <c r="J142">
         <f t="shared" si="392"/>
-        <v>0</v>
+        <v>4628.5714285714284</v>
       </c>
       <c r="K142">
         <f t="shared" si="392"/>
@@ -4704,7 +4704,7 @@
       </c>
       <c r="M142">
         <f t="shared" si="392"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.3">
@@ -4716,21 +4716,21 @@
       </c>
       <c r="C143">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44764.28571428571</v>
       </c>
       <c r="D143">
-        <v>214110</v>
-      </c>
-      <c r="H143">
-        <v>110000</v>
+        <v>274950</v>
+      </c>
+      <c r="E143">
+        <v>38400</v>
       </c>
       <c r="I143">
         <f t="shared" ref="I143" si="393">D143/7</f>
-        <v>30587.142857142859</v>
+        <v>39278.571428571428</v>
       </c>
       <c r="J143">
         <f t="shared" ref="J143" si="394">E143/7</f>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K143">
         <f t="shared" ref="K143" si="395">F143/7</f>
@@ -4742,7 +4742,7 @@
       </c>
       <c r="M143">
         <f t="shared" ref="M143" si="397">H143/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.3">
@@ -4751,15 +4751,15 @@
       </c>
       <c r="C144">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44764.28571428571</v>
       </c>
       <c r="I144">
         <f t="shared" ref="I144" si="398">D143/7</f>
-        <v>30587.142857142859</v>
+        <v>39278.571428571428</v>
       </c>
       <c r="J144">
         <f t="shared" ref="J144" si="399">E143/7</f>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K144">
         <f t="shared" ref="K144" si="400">F143/7</f>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="M144">
         <f t="shared" ref="M144" si="402">H143/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.3">
@@ -4780,15 +4780,15 @@
       </c>
       <c r="C145">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44764.28571428571</v>
       </c>
       <c r="I145">
         <f t="shared" ref="I145:M145" si="403">D143/7</f>
-        <v>30587.142857142859</v>
+        <v>39278.571428571428</v>
       </c>
       <c r="J145">
         <f t="shared" si="403"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K145">
         <f t="shared" si="403"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="M145">
         <f t="shared" si="403"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.3">
@@ -4809,15 +4809,15 @@
       </c>
       <c r="C146">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44764.28571428571</v>
       </c>
       <c r="I146">
         <f t="shared" ref="I146:M146" si="404">D143/7</f>
-        <v>30587.142857142859</v>
+        <v>39278.571428571428</v>
       </c>
       <c r="J146">
         <f t="shared" si="404"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K146">
         <f t="shared" si="404"/>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="M146">
         <f t="shared" si="404"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.3">
@@ -4838,15 +4838,15 @@
       </c>
       <c r="C147">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44764.28571428571</v>
       </c>
       <c r="I147">
         <f t="shared" ref="I147:M147" si="405">D143/7</f>
-        <v>30587.142857142859</v>
+        <v>39278.571428571428</v>
       </c>
       <c r="J147">
         <f t="shared" si="405"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K147">
         <f t="shared" si="405"/>
@@ -4858,7 +4858,7 @@
       </c>
       <c r="M147">
         <f t="shared" si="405"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.3">
@@ -4867,15 +4867,15 @@
       </c>
       <c r="C148">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44764.28571428571</v>
       </c>
       <c r="I148">
         <f t="shared" ref="I148:M148" si="406">D143/7</f>
-        <v>30587.142857142859</v>
+        <v>39278.571428571428</v>
       </c>
       <c r="J148">
         <f t="shared" si="406"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K148">
         <f t="shared" si="406"/>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="M148">
         <f t="shared" si="406"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.3">
@@ -4896,15 +4896,15 @@
       </c>
       <c r="C149">
         <f t="shared" si="373"/>
-        <v>46301.428571428572</v>
+        <v>44764.28571428571</v>
       </c>
       <c r="I149">
         <f t="shared" ref="I149:M149" si="407">D143/7</f>
-        <v>30587.142857142859</v>
+        <v>39278.571428571428</v>
       </c>
       <c r="J149">
         <f t="shared" si="407"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K149">
         <f t="shared" si="407"/>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="M149">
         <f t="shared" si="407"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.3">
@@ -4928,21 +4928,21 @@
       </c>
       <c r="C150">
         <f t="shared" si="373"/>
-        <v>58837.142857142855</v>
+        <v>59141.428571428565</v>
       </c>
       <c r="D150">
-        <v>301860</v>
-      </c>
-      <c r="H150">
-        <v>110000</v>
+        <v>382590</v>
+      </c>
+      <c r="E150">
+        <v>31400</v>
       </c>
       <c r="I150">
         <f t="shared" ref="I150" si="408">D150/7</f>
-        <v>43122.857142857145</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J150">
         <f t="shared" ref="J150" si="409">E150/7</f>
-        <v>0</v>
+        <v>4485.7142857142853</v>
       </c>
       <c r="K150">
         <f t="shared" ref="K150" si="410">F150/7</f>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="M150">
         <f t="shared" ref="M150" si="412">H150/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.3">
@@ -4963,15 +4963,15 @@
       </c>
       <c r="C151">
         <f t="shared" si="373"/>
-        <v>58837.142857142855</v>
+        <v>59141.428571428565</v>
       </c>
       <c r="I151">
         <f t="shared" ref="I151" si="413">D150/7</f>
-        <v>43122.857142857145</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J151">
         <f t="shared" ref="J151" si="414">E150/7</f>
-        <v>0</v>
+        <v>4485.7142857142853</v>
       </c>
       <c r="K151">
         <f t="shared" ref="K151" si="415">F150/7</f>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="M151">
         <f t="shared" ref="M151" si="417">H150/7</f>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.3">
@@ -4992,15 +4992,15 @@
       </c>
       <c r="C152">
         <f t="shared" si="373"/>
-        <v>58837.142857142855</v>
+        <v>59141.428571428565</v>
       </c>
       <c r="I152">
         <f t="shared" ref="I152:M152" si="418">D150/7</f>
-        <v>43122.857142857145</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J152">
         <f t="shared" si="418"/>
-        <v>0</v>
+        <v>4485.7142857142853</v>
       </c>
       <c r="K152">
         <f t="shared" si="418"/>
@@ -5012,7 +5012,7 @@
       </c>
       <c r="M152">
         <f t="shared" si="418"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.3">
@@ -5021,15 +5021,15 @@
       </c>
       <c r="C153">
         <f t="shared" si="373"/>
-        <v>58837.142857142855</v>
+        <v>59141.428571428565</v>
       </c>
       <c r="I153">
         <f t="shared" ref="I153:M153" si="419">D150/7</f>
-        <v>43122.857142857145</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J153">
         <f t="shared" si="419"/>
-        <v>0</v>
+        <v>4485.7142857142853</v>
       </c>
       <c r="K153">
         <f t="shared" si="419"/>
@@ -5041,7 +5041,7 @@
       </c>
       <c r="M153">
         <f t="shared" si="419"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.3">
@@ -5050,15 +5050,15 @@
       </c>
       <c r="C154">
         <f t="shared" si="373"/>
-        <v>58837.142857142855</v>
+        <v>59141.428571428565</v>
       </c>
       <c r="I154">
         <f t="shared" ref="I154:M154" si="420">D150/7</f>
-        <v>43122.857142857145</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J154">
         <f t="shared" si="420"/>
-        <v>0</v>
+        <v>4485.7142857142853</v>
       </c>
       <c r="K154">
         <f t="shared" si="420"/>
@@ -5070,7 +5070,7 @@
       </c>
       <c r="M154">
         <f t="shared" si="420"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.3">
@@ -5079,15 +5079,15 @@
       </c>
       <c r="C155">
         <f t="shared" si="373"/>
-        <v>58837.142857142855</v>
+        <v>59141.428571428565</v>
       </c>
       <c r="I155">
         <f t="shared" ref="I155:M155" si="421">D150/7</f>
-        <v>43122.857142857145</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J155">
         <f t="shared" si="421"/>
-        <v>0</v>
+        <v>4485.7142857142853</v>
       </c>
       <c r="K155">
         <f t="shared" si="421"/>
@@ -5099,7 +5099,7 @@
       </c>
       <c r="M155">
         <f t="shared" si="421"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.3">
@@ -5108,15 +5108,15 @@
       </c>
       <c r="C156">
         <f t="shared" si="373"/>
-        <v>58837.142857142855</v>
+        <v>59141.428571428565</v>
       </c>
       <c r="I156">
         <f t="shared" ref="I156:M156" si="422">D150/7</f>
-        <v>43122.857142857145</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J156">
         <f t="shared" si="422"/>
-        <v>0</v>
+        <v>4485.7142857142853</v>
       </c>
       <c r="K156">
         <f t="shared" si="422"/>
@@ -5128,7 +5128,7 @@
       </c>
       <c r="M156">
         <f t="shared" si="422"/>
-        <v>15714.285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.3">
@@ -5140,18 +5140,24 @@
       </c>
       <c r="C157">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>80815.28571428571</v>
+      </c>
+      <c r="D157">
+        <v>388440</v>
+      </c>
+      <c r="E157">
+        <v>38400</v>
       </c>
       <c r="H157">
-        <v>787560</v>
+        <v>138867</v>
       </c>
       <c r="I157">
         <f t="shared" ref="I157" si="423">D157/7</f>
-        <v>0</v>
+        <v>55491.428571428572</v>
       </c>
       <c r="J157">
         <f t="shared" ref="J157" si="424">E157/7</f>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K157">
         <f t="shared" ref="K157" si="425">F157/7</f>
@@ -5163,7 +5169,7 @@
       </c>
       <c r="M157">
         <f t="shared" ref="M157" si="427">H157/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.3">
@@ -5172,15 +5178,15 @@
       </c>
       <c r="C158">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>80815.28571428571</v>
       </c>
       <c r="I158">
         <f t="shared" ref="I158" si="428">D157/7</f>
-        <v>0</v>
+        <v>55491.428571428572</v>
       </c>
       <c r="J158">
         <f t="shared" ref="J158" si="429">E157/7</f>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K158">
         <f t="shared" ref="K158" si="430">F157/7</f>
@@ -5192,7 +5198,7 @@
       </c>
       <c r="M158">
         <f t="shared" ref="M158" si="432">H157/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.3">
@@ -5201,15 +5207,15 @@
       </c>
       <c r="C159">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>80815.28571428571</v>
       </c>
       <c r="I159">
         <f t="shared" ref="I159:M159" si="433">D157/7</f>
-        <v>0</v>
+        <v>55491.428571428572</v>
       </c>
       <c r="J159">
         <f t="shared" si="433"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K159">
         <f t="shared" si="433"/>
@@ -5221,7 +5227,7 @@
       </c>
       <c r="M159">
         <f t="shared" si="433"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.3">
@@ -5230,15 +5236,15 @@
       </c>
       <c r="C160">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>80815.28571428571</v>
       </c>
       <c r="I160">
         <f t="shared" ref="I160:M160" si="434">D157/7</f>
-        <v>0</v>
+        <v>55491.428571428572</v>
       </c>
       <c r="J160">
         <f t="shared" si="434"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K160">
         <f t="shared" si="434"/>
@@ -5250,7 +5256,7 @@
       </c>
       <c r="M160">
         <f t="shared" si="434"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.3">
@@ -5259,15 +5265,15 @@
       </c>
       <c r="C161">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>80815.28571428571</v>
       </c>
       <c r="I161">
         <f t="shared" ref="I161:M161" si="435">D157/7</f>
-        <v>0</v>
+        <v>55491.428571428572</v>
       </c>
       <c r="J161">
         <f t="shared" si="435"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K161">
         <f t="shared" si="435"/>
@@ -5279,7 +5285,7 @@
       </c>
       <c r="M161">
         <f t="shared" si="435"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.3">
@@ -5288,15 +5294,15 @@
       </c>
       <c r="C162">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>80815.28571428571</v>
       </c>
       <c r="I162">
         <f t="shared" ref="I162:M162" si="436">D157/7</f>
-        <v>0</v>
+        <v>55491.428571428572</v>
       </c>
       <c r="J162">
         <f t="shared" si="436"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K162">
         <f t="shared" si="436"/>
@@ -5308,7 +5314,7 @@
       </c>
       <c r="M162">
         <f t="shared" si="436"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.3">
@@ -5317,15 +5323,15 @@
       </c>
       <c r="C163">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>80815.28571428571</v>
       </c>
       <c r="I163">
         <f t="shared" ref="I163:M163" si="437">D157/7</f>
-        <v>0</v>
+        <v>55491.428571428572</v>
       </c>
       <c r="J163">
         <f t="shared" si="437"/>
-        <v>0</v>
+        <v>5485.7142857142853</v>
       </c>
       <c r="K163">
         <f t="shared" si="437"/>
@@ -5337,7 +5343,7 @@
       </c>
       <c r="M163">
         <f t="shared" si="437"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.3">
@@ -5349,18 +5355,24 @@
       </c>
       <c r="C164">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79108.142857142855</v>
+      </c>
+      <c r="D164">
+        <v>382590</v>
+      </c>
+      <c r="E164">
+        <v>32300</v>
       </c>
       <c r="H164">
-        <v>787560</v>
+        <v>138867</v>
       </c>
       <c r="I164">
         <f t="shared" ref="I164" si="438">D164/7</f>
-        <v>0</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J164">
         <f t="shared" ref="J164" si="439">E164/7</f>
-        <v>0</v>
+        <v>4614.2857142857147</v>
       </c>
       <c r="K164">
         <f t="shared" ref="K164" si="440">F164/7</f>
@@ -5372,7 +5384,7 @@
       </c>
       <c r="M164">
         <f t="shared" ref="M164" si="442">H164/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.3">
@@ -5381,15 +5393,15 @@
       </c>
       <c r="C165">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79108.142857142855</v>
       </c>
       <c r="I165">
         <f t="shared" ref="I165" si="443">D164/7</f>
-        <v>0</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J165">
         <f t="shared" ref="J165" si="444">E164/7</f>
-        <v>0</v>
+        <v>4614.2857142857147</v>
       </c>
       <c r="K165">
         <f t="shared" ref="K165" si="445">F164/7</f>
@@ -5401,7 +5413,7 @@
       </c>
       <c r="M165">
         <f t="shared" ref="M165" si="447">H164/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.3">
@@ -5410,15 +5422,15 @@
       </c>
       <c r="C166">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79108.142857142855</v>
       </c>
       <c r="I166">
         <f t="shared" ref="I166:M166" si="448">D164/7</f>
-        <v>0</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J166">
         <f t="shared" si="448"/>
-        <v>0</v>
+        <v>4614.2857142857147</v>
       </c>
       <c r="K166">
         <f t="shared" si="448"/>
@@ -5430,7 +5442,7 @@
       </c>
       <c r="M166">
         <f t="shared" si="448"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.3">
@@ -5439,15 +5451,15 @@
       </c>
       <c r="C167">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79108.142857142855</v>
       </c>
       <c r="I167">
         <f t="shared" ref="I167:M167" si="449">D164/7</f>
-        <v>0</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J167">
         <f t="shared" si="449"/>
-        <v>0</v>
+        <v>4614.2857142857147</v>
       </c>
       <c r="K167">
         <f t="shared" si="449"/>
@@ -5459,7 +5471,7 @@
       </c>
       <c r="M167">
         <f t="shared" si="449"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.3">
@@ -5468,15 +5480,15 @@
       </c>
       <c r="C168">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79108.142857142855</v>
       </c>
       <c r="I168">
         <f t="shared" ref="I168:M168" si="450">D164/7</f>
-        <v>0</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J168">
         <f t="shared" si="450"/>
-        <v>0</v>
+        <v>4614.2857142857147</v>
       </c>
       <c r="K168">
         <f t="shared" si="450"/>
@@ -5488,7 +5500,7 @@
       </c>
       <c r="M168">
         <f t="shared" si="450"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.3">
@@ -5497,15 +5509,15 @@
       </c>
       <c r="C169">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79108.142857142855</v>
       </c>
       <c r="I169">
         <f t="shared" ref="I169:M169" si="451">D164/7</f>
-        <v>0</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J169">
         <f t="shared" si="451"/>
-        <v>0</v>
+        <v>4614.2857142857147</v>
       </c>
       <c r="K169">
         <f t="shared" si="451"/>
@@ -5517,7 +5529,7 @@
       </c>
       <c r="M169">
         <f t="shared" si="451"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.3">
@@ -5526,15 +5538,15 @@
       </c>
       <c r="C170">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79108.142857142855</v>
       </c>
       <c r="I170">
         <f t="shared" ref="I170:M170" si="452">D164/7</f>
-        <v>0</v>
+        <v>54655.714285714283</v>
       </c>
       <c r="J170">
         <f t="shared" si="452"/>
-        <v>0</v>
+        <v>4614.2857142857147</v>
       </c>
       <c r="K170">
         <f t="shared" si="452"/>
@@ -5546,7 +5558,7 @@
       </c>
       <c r="M170">
         <f t="shared" si="452"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.3">
@@ -5558,18 +5570,24 @@
       </c>
       <c r="C171">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>81782.428571428565</v>
+      </c>
+      <c r="D171">
+        <v>389610</v>
+      </c>
+      <c r="E171">
+        <v>44000</v>
       </c>
       <c r="H171">
-        <v>787560</v>
+        <v>138867</v>
       </c>
       <c r="I171">
         <f t="shared" ref="I171" si="453">D171/7</f>
-        <v>0</v>
+        <v>55658.571428571428</v>
       </c>
       <c r="J171">
         <f t="shared" ref="J171" si="454">E171/7</f>
-        <v>0</v>
+        <v>6285.7142857142853</v>
       </c>
       <c r="K171">
         <f t="shared" ref="K171" si="455">F171/7</f>
@@ -5581,7 +5599,7 @@
       </c>
       <c r="M171">
         <f t="shared" ref="M171" si="457">H171/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.3">
@@ -5590,15 +5608,15 @@
       </c>
       <c r="C172">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>81782.428571428565</v>
       </c>
       <c r="I172">
         <f t="shared" ref="I172" si="458">D171/7</f>
-        <v>0</v>
+        <v>55658.571428571428</v>
       </c>
       <c r="J172">
         <f t="shared" ref="J172" si="459">E171/7</f>
-        <v>0</v>
+        <v>6285.7142857142853</v>
       </c>
       <c r="K172">
         <f t="shared" ref="K172" si="460">F171/7</f>
@@ -5610,7 +5628,7 @@
       </c>
       <c r="M172">
         <f t="shared" ref="M172" si="462">H171/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.3">
@@ -5619,15 +5637,15 @@
       </c>
       <c r="C173">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>81782.428571428565</v>
       </c>
       <c r="I173">
         <f t="shared" ref="I173:M173" si="463">D171/7</f>
-        <v>0</v>
+        <v>55658.571428571428</v>
       </c>
       <c r="J173">
         <f t="shared" si="463"/>
-        <v>0</v>
+        <v>6285.7142857142853</v>
       </c>
       <c r="K173">
         <f t="shared" si="463"/>
@@ -5639,7 +5657,7 @@
       </c>
       <c r="M173">
         <f t="shared" si="463"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.3">
@@ -5648,15 +5666,15 @@
       </c>
       <c r="C174">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>81782.428571428565</v>
       </c>
       <c r="I174">
         <f t="shared" ref="I174:M174" si="464">D171/7</f>
-        <v>0</v>
+        <v>55658.571428571428</v>
       </c>
       <c r="J174">
         <f t="shared" si="464"/>
-        <v>0</v>
+        <v>6285.7142857142853</v>
       </c>
       <c r="K174">
         <f t="shared" si="464"/>
@@ -5668,7 +5686,7 @@
       </c>
       <c r="M174">
         <f t="shared" si="464"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.3">
@@ -5677,15 +5695,15 @@
       </c>
       <c r="C175">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>81782.428571428565</v>
       </c>
       <c r="I175">
         <f t="shared" ref="I175:M175" si="465">D171/7</f>
-        <v>0</v>
+        <v>55658.571428571428</v>
       </c>
       <c r="J175">
         <f t="shared" si="465"/>
-        <v>0</v>
+        <v>6285.7142857142853</v>
       </c>
       <c r="K175">
         <f t="shared" si="465"/>
@@ -5697,7 +5715,7 @@
       </c>
       <c r="M175">
         <f t="shared" si="465"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.3">
@@ -5706,15 +5724,15 @@
       </c>
       <c r="C176">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>81782.428571428565</v>
       </c>
       <c r="I176">
         <f t="shared" ref="I176:M176" si="466">D171/7</f>
-        <v>0</v>
+        <v>55658.571428571428</v>
       </c>
       <c r="J176">
         <f t="shared" si="466"/>
-        <v>0</v>
+        <v>6285.7142857142853</v>
       </c>
       <c r="K176">
         <f t="shared" si="466"/>
@@ -5726,7 +5744,7 @@
       </c>
       <c r="M176">
         <f t="shared" si="466"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.3">
@@ -5735,15 +5753,15 @@
       </c>
       <c r="C177">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>81782.428571428565</v>
       </c>
       <c r="I177">
         <f t="shared" ref="I177:M177" si="467">D171/7</f>
-        <v>0</v>
+        <v>55658.571428571428</v>
       </c>
       <c r="J177">
         <f t="shared" si="467"/>
-        <v>0</v>
+        <v>6285.7142857142853</v>
       </c>
       <c r="K177">
         <f t="shared" si="467"/>
@@ -5755,7 +5773,7 @@
       </c>
       <c r="M177">
         <f t="shared" si="467"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.3">
@@ -5767,18 +5785,24 @@
       </c>
       <c r="C178">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79932.42857142858</v>
+      </c>
+      <c r="D178">
+        <v>383760</v>
+      </c>
+      <c r="E178">
+        <v>36900</v>
       </c>
       <c r="H178">
-        <v>787560</v>
+        <v>138867</v>
       </c>
       <c r="I178">
         <f t="shared" ref="I178" si="468">D178/7</f>
-        <v>0</v>
+        <v>54822.857142857145</v>
       </c>
       <c r="J178">
         <f t="shared" ref="J178" si="469">E178/7</f>
-        <v>0</v>
+        <v>5271.4285714285716</v>
       </c>
       <c r="K178">
         <f t="shared" ref="K178" si="470">F178/7</f>
@@ -5790,7 +5814,7 @@
       </c>
       <c r="M178">
         <f t="shared" ref="M178" si="472">H178/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.3">
@@ -5799,15 +5823,15 @@
       </c>
       <c r="C179">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79932.42857142858</v>
       </c>
       <c r="I179">
         <f t="shared" ref="I179" si="473">D178/7</f>
-        <v>0</v>
+        <v>54822.857142857145</v>
       </c>
       <c r="J179">
         <f t="shared" ref="J179" si="474">E178/7</f>
-        <v>0</v>
+        <v>5271.4285714285716</v>
       </c>
       <c r="K179">
         <f t="shared" ref="K179" si="475">F178/7</f>
@@ -5819,7 +5843,7 @@
       </c>
       <c r="M179">
         <f t="shared" ref="M179" si="477">H178/7</f>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.3">
@@ -5828,15 +5852,15 @@
       </c>
       <c r="C180">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79932.42857142858</v>
       </c>
       <c r="I180">
         <f t="shared" ref="I180:M180" si="478">D178/7</f>
-        <v>0</v>
+        <v>54822.857142857145</v>
       </c>
       <c r="J180">
         <f t="shared" si="478"/>
-        <v>0</v>
+        <v>5271.4285714285716</v>
       </c>
       <c r="K180">
         <f t="shared" si="478"/>
@@ -5848,7 +5872,7 @@
       </c>
       <c r="M180">
         <f t="shared" si="478"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.3">
@@ -5857,15 +5881,15 @@
       </c>
       <c r="C181">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79932.42857142858</v>
       </c>
       <c r="I181">
         <f t="shared" ref="I181:M181" si="479">D178/7</f>
-        <v>0</v>
+        <v>54822.857142857145</v>
       </c>
       <c r="J181">
         <f t="shared" si="479"/>
-        <v>0</v>
+        <v>5271.4285714285716</v>
       </c>
       <c r="K181">
         <f t="shared" si="479"/>
@@ -5877,7 +5901,7 @@
       </c>
       <c r="M181">
         <f t="shared" si="479"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.3">
@@ -5886,15 +5910,15 @@
       </c>
       <c r="C182">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79932.42857142858</v>
       </c>
       <c r="I182">
         <f t="shared" ref="I182:M182" si="480">D178/7</f>
-        <v>0</v>
+        <v>54822.857142857145</v>
       </c>
       <c r="J182">
         <f t="shared" si="480"/>
-        <v>0</v>
+        <v>5271.4285714285716</v>
       </c>
       <c r="K182">
         <f t="shared" si="480"/>
@@ -5906,7 +5930,7 @@
       </c>
       <c r="M182">
         <f t="shared" si="480"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.3">
@@ -5915,15 +5939,15 @@
       </c>
       <c r="C183">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79932.42857142858</v>
       </c>
       <c r="I183">
         <f t="shared" ref="I183:M183" si="481">D178/7</f>
-        <v>0</v>
+        <v>54822.857142857145</v>
       </c>
       <c r="J183">
         <f t="shared" si="481"/>
-        <v>0</v>
+        <v>5271.4285714285716</v>
       </c>
       <c r="K183">
         <f t="shared" si="481"/>
@@ -5935,7 +5959,7 @@
       </c>
       <c r="M183">
         <f t="shared" si="481"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.3">
@@ -5944,15 +5968,15 @@
       </c>
       <c r="C184">
         <f t="shared" si="373"/>
-        <v>112508.57142857143</v>
+        <v>79932.42857142858</v>
       </c>
       <c r="I184">
         <f t="shared" ref="I184:M184" si="482">D178/7</f>
-        <v>0</v>
+        <v>54822.857142857145</v>
       </c>
       <c r="J184">
         <f t="shared" si="482"/>
-        <v>0</v>
+        <v>5271.4285714285716</v>
       </c>
       <c r="K184">
         <f t="shared" si="482"/>
@@ -5964,7 +5988,7 @@
       </c>
       <c r="M184">
         <f t="shared" si="482"/>
-        <v>112508.57142857143</v>
+        <v>19838.142857142859</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.3">
@@ -5976,10 +6000,10 @@
       </c>
       <c r="C185">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="H185">
-        <v>1156000</v>
+        <v>683383</v>
       </c>
       <c r="I185">
         <f t="shared" ref="I185" si="483">D185/7</f>
@@ -5999,7 +6023,7 @@
       </c>
       <c r="M185">
         <f t="shared" ref="M185" si="487">H185/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.3">
@@ -6008,7 +6032,7 @@
       </c>
       <c r="C186">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I186">
         <f t="shared" ref="I186" si="488">D185/7</f>
@@ -6028,7 +6052,7 @@
       </c>
       <c r="M186">
         <f t="shared" ref="M186" si="492">H185/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.3">
@@ -6037,7 +6061,7 @@
       </c>
       <c r="C187">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I187">
         <f t="shared" ref="I187:M187" si="493">D185/7</f>
@@ -6057,7 +6081,7 @@
       </c>
       <c r="M187">
         <f t="shared" si="493"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.3">
@@ -6066,7 +6090,7 @@
       </c>
       <c r="C188">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I188">
         <f t="shared" ref="I188:M188" si="494">D185/7</f>
@@ -6086,7 +6110,7 @@
       </c>
       <c r="M188">
         <f t="shared" si="494"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.3">
@@ -6095,7 +6119,7 @@
       </c>
       <c r="C189">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I189">
         <f t="shared" ref="I189:M189" si="495">D185/7</f>
@@ -6115,7 +6139,7 @@
       </c>
       <c r="M189">
         <f t="shared" si="495"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.3">
@@ -6124,7 +6148,7 @@
       </c>
       <c r="C190">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I190">
         <f t="shared" ref="I190:M190" si="496">D185/7</f>
@@ -6144,7 +6168,7 @@
       </c>
       <c r="M190">
         <f t="shared" si="496"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.3">
@@ -6153,7 +6177,7 @@
       </c>
       <c r="C191">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I191">
         <f t="shared" ref="I191:M191" si="497">D185/7</f>
@@ -6173,7 +6197,7 @@
       </c>
       <c r="M191">
         <f t="shared" si="497"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.3">
@@ -6185,10 +6209,10 @@
       </c>
       <c r="C192">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="H192">
-        <v>1156000</v>
+        <v>683383</v>
       </c>
       <c r="I192">
         <f t="shared" ref="I192" si="498">D192/7</f>
@@ -6208,7 +6232,7 @@
       </c>
       <c r="M192">
         <f t="shared" ref="M192" si="502">H192/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.3">
@@ -6217,7 +6241,7 @@
       </c>
       <c r="C193">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I193">
         <f t="shared" ref="I193" si="503">D192/7</f>
@@ -6237,7 +6261,7 @@
       </c>
       <c r="M193">
         <f t="shared" ref="M193" si="507">H192/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.3">
@@ -6246,7 +6270,7 @@
       </c>
       <c r="C194">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I194">
         <f t="shared" ref="I194:M194" si="508">D192/7</f>
@@ -6266,7 +6290,7 @@
       </c>
       <c r="M194">
         <f t="shared" si="508"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.3">
@@ -6275,7 +6299,7 @@
       </c>
       <c r="C195">
         <f t="shared" si="373"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I195">
         <f t="shared" ref="I195:M195" si="509">D192/7</f>
@@ -6295,7 +6319,7 @@
       </c>
       <c r="M195">
         <f t="shared" si="509"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.3">
@@ -6304,7 +6328,7 @@
       </c>
       <c r="C196">
         <f t="shared" ref="C196:C212" si="510">SUM(I196:M196)</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I196">
         <f t="shared" ref="I196:M196" si="511">D192/7</f>
@@ -6324,7 +6348,7 @@
       </c>
       <c r="M196">
         <f t="shared" si="511"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.3">
@@ -6333,7 +6357,7 @@
       </c>
       <c r="C197">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I197">
         <f t="shared" ref="I197:M197" si="512">D192/7</f>
@@ -6353,7 +6377,7 @@
       </c>
       <c r="M197">
         <f t="shared" si="512"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.3">
@@ -6362,7 +6386,7 @@
       </c>
       <c r="C198">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I198">
         <f t="shared" ref="I198:M198" si="513">D192/7</f>
@@ -6382,7 +6406,7 @@
       </c>
       <c r="M198">
         <f t="shared" si="513"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.3">
@@ -6394,10 +6418,10 @@
       </c>
       <c r="C199">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="H199">
-        <v>1156000</v>
+        <v>683383</v>
       </c>
       <c r="I199">
         <f t="shared" ref="I199" si="514">D199/7</f>
@@ -6417,7 +6441,7 @@
       </c>
       <c r="M199">
         <f t="shared" ref="M199" si="518">H199/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.3">
@@ -6426,7 +6450,7 @@
       </c>
       <c r="C200">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I200">
         <f t="shared" ref="I200" si="519">D199/7</f>
@@ -6446,7 +6470,7 @@
       </c>
       <c r="M200">
         <f t="shared" ref="M200" si="523">H199/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.3">
@@ -6455,7 +6479,7 @@
       </c>
       <c r="C201">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I201">
         <f t="shared" ref="I201:M201" si="524">D199/7</f>
@@ -6475,7 +6499,7 @@
       </c>
       <c r="M201">
         <f t="shared" si="524"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.3">
@@ -6484,7 +6508,7 @@
       </c>
       <c r="C202">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I202">
         <f t="shared" ref="I202:M202" si="525">D199/7</f>
@@ -6504,7 +6528,7 @@
       </c>
       <c r="M202">
         <f t="shared" si="525"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.3">
@@ -6513,7 +6537,7 @@
       </c>
       <c r="C203">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I203">
         <f t="shared" ref="I203:M203" si="526">D199/7</f>
@@ -6533,7 +6557,7 @@
       </c>
       <c r="M203">
         <f t="shared" si="526"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.3">
@@ -6542,7 +6566,7 @@
       </c>
       <c r="C204">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I204">
         <f t="shared" ref="I204:M204" si="527">D199/7</f>
@@ -6562,7 +6586,7 @@
       </c>
       <c r="M204">
         <f t="shared" si="527"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.3">
@@ -6571,7 +6595,7 @@
       </c>
       <c r="C205">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I205">
         <f t="shared" ref="I205:M205" si="528">D199/7</f>
@@ -6591,7 +6615,7 @@
       </c>
       <c r="M205">
         <f t="shared" si="528"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.3">
@@ -6603,10 +6627,10 @@
       </c>
       <c r="C206">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="H206">
-        <v>1156000</v>
+        <v>683383</v>
       </c>
       <c r="I206">
         <f t="shared" ref="I206" si="529">D206/7</f>
@@ -6626,7 +6650,7 @@
       </c>
       <c r="M206">
         <f t="shared" ref="M206" si="533">H206/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.3">
@@ -6635,7 +6659,7 @@
       </c>
       <c r="C207">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I207">
         <f t="shared" ref="I207" si="534">D206/7</f>
@@ -6655,7 +6679,7 @@
       </c>
       <c r="M207">
         <f t="shared" ref="M207" si="538">H206/7</f>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.3">
@@ -6664,7 +6688,7 @@
       </c>
       <c r="C208">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I208">
         <f t="shared" ref="I208:M208" si="539">D206/7</f>
@@ -6684,7 +6708,7 @@
       </c>
       <c r="M208">
         <f t="shared" si="539"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.3">
@@ -6693,7 +6717,7 @@
       </c>
       <c r="C209">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I209">
         <f t="shared" ref="I209:M209" si="540">D206/7</f>
@@ -6713,7 +6737,7 @@
       </c>
       <c r="M209">
         <f t="shared" si="540"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.3">
@@ -6722,7 +6746,7 @@
       </c>
       <c r="C210">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I210">
         <f t="shared" ref="I210:M210" si="541">D206/7</f>
@@ -6742,7 +6766,7 @@
       </c>
       <c r="M210">
         <f t="shared" si="541"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.3">
@@ -6751,7 +6775,7 @@
       </c>
       <c r="C211">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I211">
         <f t="shared" ref="I211:M211" si="542">D206/7</f>
@@ -6771,7 +6795,7 @@
       </c>
       <c r="M211">
         <f t="shared" si="542"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.3">
@@ -6780,7 +6804,7 @@
       </c>
       <c r="C212">
         <f t="shared" si="510"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
       <c r="I212">
         <f t="shared" ref="I212:M212" si="543">D206/7</f>
@@ -6800,7 +6824,7 @@
       </c>
       <c r="M212">
         <f t="shared" si="543"/>
-        <v>165142.85714285713</v>
+        <v>97626.142857142855</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>